<commit_message>
Add Q222 financial data to existing model (limited)
</commit_message>
<xml_diff>
--- a/$ANF.xlsx
+++ b/$ANF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465CB485-E78F-466F-A19D-F576BE704EB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A322973-9214-9841-AFC1-B18D6B12C798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="18900" xr2:uid="{BED0471A-CBC0-4084-A037-CD3E53E820DA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18900" xr2:uid="{BED0471A-CBC0-4084-A037-CD3E53E820DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="140">
   <si>
     <t>$ANF</t>
   </si>
@@ -656,7 +666,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -739,6 +749,13 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -782,7 +799,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -867,16 +884,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -891,8 +908,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10248900" y="19050"/>
-          <a:ext cx="0" cy="11220450"/>
+          <a:off x="12430125" y="6350"/>
+          <a:ext cx="0" cy="12760325"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1268,55 +1285,55 @@
   <dimension ref="B2:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C26" sqref="C26:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="H5" s="44" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="H5" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="46"/>
-      <c r="S5" s="44" t="s">
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="49"/>
+      <c r="S5" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="46"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="49"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8">
-        <v>15.88</v>
+        <v>17.739999999999998</v>
       </c>
       <c r="D6" s="14"/>
       <c r="H6" s="41">
@@ -1339,15 +1356,17 @@
       <c r="V6" s="8"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="16">
-        <v>50.446862000000003</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>42</v>
+        <f>'Financial Model'!P20</f>
+        <v>50.441000000000003</v>
+      </c>
+      <c r="D7" s="14" t="str">
+        <f>$C$27</f>
+        <v>Q222</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="8"/>
@@ -1365,13 +1384,13 @@
       <c r="V7" s="8"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="16">
         <f>C6*C7</f>
-        <v>801.09616856000014</v>
+        <v>894.82333999999992</v>
       </c>
       <c r="D8" s="14"/>
       <c r="H8" s="6" t="s">
@@ -1392,15 +1411,17 @@
       <c r="V8" s="8"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="16">
-        <v>468.4</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>42</v>
+        <f>'Financial Model'!P39</f>
+        <v>369.95600000000002</v>
+      </c>
+      <c r="D9" s="14" t="str">
+        <f t="shared" ref="D9:D11" si="0">$C$27</f>
+        <v>Q222</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="42" t="s">
@@ -1420,15 +1441,17 @@
       <c r="V9" s="8"/>
       <c r="W9" s="9"/>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="16">
-        <v>303.89999999999998</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>42</v>
+        <f>'Financial Model'!P55</f>
+        <v>304.21899999999999</v>
+      </c>
+      <c r="D10" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Q222</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="42" t="s">
@@ -1448,16 +1471,17 @@
       <c r="V10" s="8"/>
       <c r="W10" s="9"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="16">
         <f>C9-C10</f>
-        <v>164.5</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>42</v>
+        <v>65.737000000000023</v>
+      </c>
+      <c r="D11" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Q222</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="42" t="s">
@@ -1475,13 +1499,13 @@
       <c r="V11" s="8"/>
       <c r="W11" s="9"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="17">
         <f>C8-C11</f>
-        <v>636.59616856000014</v>
+        <v>829.08633999999984</v>
       </c>
       <c r="D12" s="15"/>
       <c r="H12" s="6"/>
@@ -1500,7 +1524,7 @@
       <c r="V12" s="8"/>
       <c r="W12" s="9"/>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.15">
       <c r="H13" s="6"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -1517,7 +1541,7 @@
       <c r="V13" s="8"/>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.15">
       <c r="H14" s="41">
         <v>44136</v>
       </c>
@@ -1536,12 +1560,12 @@
       <c r="V14" s="8"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="44" t="s">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B15" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
       <c r="H15" s="6"/>
       <c r="I15" s="42" t="s">
         <v>138</v>
@@ -1560,14 +1584,14 @@
       <c r="V15" s="8"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="50"/>
+      <c r="D16" s="53"/>
       <c r="H16" s="6"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1584,14 +1608,14 @@
       <c r="V16" s="8"/>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="50"/>
+      <c r="D17" s="53"/>
       <c r="H17" s="6"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1608,14 +1632,14 @@
       <c r="V17" s="8"/>
       <c r="W17" s="9"/>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="50"/>
+      <c r="D18" s="53"/>
       <c r="H18" s="6"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1632,10 +1656,10 @@
       <c r="V18" s="8"/>
       <c r="W18" s="9"/>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B19" s="13"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
       <c r="H19" s="6"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1652,7 +1676,7 @@
       <c r="V19" s="8"/>
       <c r="W19" s="9"/>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.15">
       <c r="H20" s="7"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
@@ -1667,141 +1691,144 @@
       <c r="V20" s="10"/>
       <c r="W20" s="11"/>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B22" s="44" t="s">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B22" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="50"/>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="D23" s="53"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="52">
         <v>1892</v>
       </c>
-      <c r="D24" s="50"/>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="D24" s="53"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B25" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="49">
-        <v>728</v>
-      </c>
-      <c r="D25" s="50"/>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C25" s="52">
+        <f>'Financial Model'!P36</f>
+        <v>734</v>
+      </c>
+      <c r="D25" s="53"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B26" s="6"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C26" s="52"/>
+      <c r="D26" s="53"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="50"/>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C27" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="45">
+        <v>44798</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="48"/>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B31" s="44" t="s">
+      <c r="D28" s="51"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B31" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="46"/>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C31" s="48"/>
+      <c r="D31" s="49"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="55">
+      <c r="C32" s="58">
         <f>C6/'Financial Model'!O18</f>
-        <v>-0.96423583702713767</v>
-      </c>
-      <c r="D32" s="56"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+        <v>-1.077175299046689</v>
+      </c>
+      <c r="D32" s="59"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="51">
+      <c r="C33" s="54">
         <f>C6/'Financial Model'!O19</f>
-        <v>-50.21450968486225</v>
-      </c>
-      <c r="D33" s="52"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+        <v>-56.096058048454417</v>
+      </c>
+      <c r="D33" s="55"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="50"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="51">
-        <f>C6/'Financial Model'!O64</f>
-        <v>1.1733497350330941</v>
-      </c>
-      <c r="D35" s="52"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="54">
+        <f>C6/'Financial Model'!P64</f>
+        <v>1.3298883267742285</v>
+      </c>
+      <c r="D35" s="55"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="6"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="52"/>
+      <c r="D36" s="53"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="51">
+      <c r="C37" s="54">
         <f>C6/'Financial Model'!X19</f>
-        <v>3.5983436371240685</v>
-      </c>
-      <c r="D37" s="52"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+        <v>4.0198120983993046</v>
+      </c>
+      <c r="D37" s="55"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="51">
+      <c r="C38" s="54">
         <f>C12/'Financial Model'!X18</f>
-        <v>2.420425719782521</v>
-      </c>
-      <c r="D38" s="52"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+        <v>3.1522996844226485</v>
+      </c>
+      <c r="D38" s="55"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="54"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="23">
     <mergeCell ref="S5:W5"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
@@ -1821,7 +1848,6 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
@@ -1841,20 +1867,20 @@
   <dimension ref="B1:AI70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
@@ -1894,7 +1920,7 @@
       <c r="O1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="22" t="s">
         <v>43</v>
       </c>
       <c r="Q1" s="19" t="s">
@@ -1949,7 +1975,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="2:35" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:35" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="20"/>
       <c r="H2" s="23">
         <v>44044</v>
@@ -1972,6 +1998,9 @@
       <c r="O2" s="23">
         <v>44681</v>
       </c>
+      <c r="P2" s="23">
+        <v>44742</v>
+      </c>
       <c r="V2" s="23">
         <v>43862</v>
       </c>
@@ -1982,7 +2011,7 @@
         <v>44590</v>
       </c>
     </row>
-    <row r="3" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="34" t="s">
         <v>103</v>
       </c>
@@ -2008,6 +2037,9 @@
       <c r="O3" s="32">
         <v>428.834</v>
       </c>
+      <c r="P3" s="32">
+        <v>436.93400000000003</v>
+      </c>
       <c r="V3" s="32">
         <v>2158.5140000000001</v>
       </c>
@@ -2018,7 +2050,7 @@
         <v>2147.9789999999998</v>
       </c>
     </row>
-    <row r="4" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="34" t="s">
         <v>104</v>
       </c>
@@ -2044,6 +2076,9 @@
       <c r="O4" s="32">
         <v>383.928</v>
       </c>
+      <c r="P4" s="32">
+        <v>368.15699999999998</v>
+      </c>
       <c r="V4" s="32">
         <v>1464.559</v>
       </c>
@@ -2054,7 +2089,7 @@
         <v>1564.789</v>
       </c>
     </row>
-    <row r="5" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>60</v>
       </c>
@@ -2081,6 +2116,9 @@
       <c r="O5" s="25">
         <v>812.76199999999994</v>
       </c>
+      <c r="P5" s="25">
+        <v>805.09100000000001</v>
+      </c>
       <c r="V5" s="25">
         <f>V3+V4</f>
         <v>3623.0730000000003</v>
@@ -2094,7 +2132,7 @@
         <v>3712.768</v>
       </c>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>61</v>
       </c>
@@ -2121,6 +2159,9 @@
       <c r="O6" s="26">
         <v>363.21600000000001</v>
       </c>
+      <c r="P6" s="26">
+        <v>339.2</v>
+      </c>
       <c r="V6" s="26">
         <v>1472.155</v>
       </c>
@@ -2131,7 +2172,7 @@
         <v>1400.7729999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>62</v>
       </c>
@@ -2145,24 +2186,28 @@
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="25">
-        <f>K5-K6</f>
+        <f t="shared" ref="K7:P7" si="1">K5-K6</f>
         <v>495.13399999999996</v>
       </c>
       <c r="L7" s="25">
-        <f>L5-L6</f>
+        <f t="shared" si="1"/>
         <v>563.48500000000001</v>
       </c>
       <c r="M7" s="25">
-        <f>M5-M6</f>
+        <f t="shared" si="1"/>
         <v>576.24399999999991</v>
       </c>
       <c r="N7" s="25">
-        <f>N5-N6</f>
+        <f t="shared" si="1"/>
         <v>677.13200000000029</v>
       </c>
       <c r="O7" s="25">
-        <f>O5-O6</f>
+        <f t="shared" si="1"/>
         <v>449.54599999999994</v>
+      </c>
+      <c r="P7" s="25">
+        <f t="shared" si="1"/>
+        <v>465.89100000000002</v>
       </c>
       <c r="V7" s="25">
         <f>V5-V6</f>
@@ -2177,7 +2222,7 @@
         <v>2311.9949999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
@@ -2198,12 +2243,15 @@
         <v>351.80399999999997</v>
       </c>
       <c r="N8" s="26">
-        <f t="shared" ref="N8:N17" si="1">X8-M8-L8-K8</f>
+        <f t="shared" ref="N8:N17" si="2">X8-M8-L8-K8</f>
         <v>436.2290000000001</v>
       </c>
       <c r="O8" s="26">
         <v>337.54300000000001</v>
       </c>
+      <c r="P8" s="26">
+        <v>340.791</v>
+      </c>
       <c r="V8" s="26">
         <v>1551.2429999999999</v>
       </c>
@@ -2214,7 +2262,7 @@
         <v>1429.4760000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
@@ -2235,12 +2283,15 @@
         <v>146.26900000000001</v>
       </c>
       <c r="N9" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>145.68600000000004</v>
       </c>
       <c r="O9" s="26">
         <v>122.149</v>
       </c>
+      <c r="P9" s="26">
+        <v>124.16800000000001</v>
+      </c>
       <c r="V9" s="26">
         <v>464.61500000000001</v>
       </c>
@@ -2251,7 +2302,7 @@
         <v>536.81500000000005</v>
       </c>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
@@ -2272,12 +2323,15 @@
         <v>6.7489999999999997</v>
       </c>
       <c r="N10" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9009999999999994</v>
       </c>
       <c r="O10" s="26">
         <v>3.4220000000000002</v>
       </c>
+      <c r="P10" s="26">
+        <v>2.17</v>
+      </c>
       <c r="V10" s="26">
         <v>19.135000000000002</v>
       </c>
@@ -2288,7 +2342,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
@@ -2313,11 +2367,14 @@
         <v>-1.3090000000000002</v>
       </c>
       <c r="N11" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.8169999999999993</v>
       </c>
       <c r="O11" s="26">
         <v>-3.8420000000000001</v>
+      </c>
+      <c r="P11" s="26">
+        <v>0.95299999999999996</v>
       </c>
       <c r="V11" s="26">
         <f>47.257-1.4</f>
@@ -2332,7 +2389,7 @@
         <v>-9.48</v>
       </c>
     </row>
-    <row r="12" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>67</v>
       </c>
@@ -2346,24 +2403,28 @@
       </c>
       <c r="J12" s="25"/>
       <c r="K12" s="25">
-        <f>K7-K8-K9-K10-K11</f>
+        <f t="shared" ref="K12:P12" si="3">K7-K8-K9-K10-K11</f>
         <v>57.432999999999971</v>
       </c>
       <c r="L12" s="25">
-        <f>L7-L8-L9-L10-L11</f>
+        <f t="shared" si="3"/>
         <v>114.78700000000002</v>
       </c>
       <c r="M12" s="25">
-        <f>M7-M8-M9-M10-M11</f>
+        <f t="shared" si="3"/>
         <v>72.730999999999938</v>
       </c>
       <c r="N12" s="25">
-        <f>N7-N8-N9-N10-N11</f>
+        <f t="shared" si="3"/>
         <v>98.133000000000152</v>
       </c>
       <c r="O12" s="25">
-        <f>O7-O8-O9-O10-O11</f>
+        <f t="shared" si="3"/>
         <v>-9.7260000000000719</v>
+      </c>
+      <c r="P12" s="25">
+        <f t="shared" si="3"/>
+        <v>-2.1909999999999834</v>
       </c>
       <c r="V12" s="25">
         <f>V7-V8-V9-V10-V11</f>
@@ -2378,7 +2439,7 @@
         <v>343.08399999999972</v>
       </c>
     </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>68</v>
       </c>
@@ -2399,12 +2460,15 @@
         <v>7.27</v>
       </c>
       <c r="N13" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9589999999999996</v>
       </c>
       <c r="O13" s="26">
         <v>7.3070000000000004</v>
       </c>
+      <c r="P13" s="26">
+        <v>6.9169999999999998</v>
+      </c>
       <c r="V13" s="26">
         <v>7.7370000000000001</v>
       </c>
@@ -2415,7 +2479,7 @@
         <v>34.11</v>
       </c>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>69</v>
       </c>
@@ -2429,24 +2493,28 @@
       </c>
       <c r="J14" s="26"/>
       <c r="K14" s="26">
-        <f>K12-K13</f>
+        <f t="shared" ref="K14:P14" si="4">K12-K13</f>
         <v>48.82699999999997</v>
       </c>
       <c r="L14" s="26">
-        <f>L12-L13</f>
+        <f t="shared" si="4"/>
         <v>103.51200000000001</v>
       </c>
       <c r="M14" s="26">
-        <f>M12-M13</f>
+        <f t="shared" si="4"/>
         <v>65.460999999999942</v>
       </c>
       <c r="N14" s="26">
-        <f>N12-N13</f>
+        <f t="shared" si="4"/>
         <v>91.174000000000149</v>
       </c>
       <c r="O14" s="26">
-        <f>O12-O13</f>
+        <f t="shared" si="4"/>
         <v>-17.033000000000072</v>
+      </c>
+      <c r="P14" s="26">
+        <f t="shared" si="4"/>
+        <v>-9.1079999999999828</v>
       </c>
       <c r="V14" s="26">
         <f>V12-V13</f>
@@ -2461,7 +2529,7 @@
         <v>308.97399999999971</v>
       </c>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
@@ -2482,12 +2550,15 @@
         <v>16.382999999999999</v>
       </c>
       <c r="N15" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23.347999999999999</v>
       </c>
       <c r="O15" s="26">
         <v>-2.1869999999999998</v>
       </c>
+      <c r="P15" s="26">
+        <v>5.6340000000000003</v>
+      </c>
       <c r="V15" s="26">
         <v>17.370999999999999</v>
       </c>
@@ -2498,7 +2569,7 @@
         <v>38.908000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
@@ -2512,24 +2583,28 @@
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="25">
-        <f>K14-K15</f>
+        <f t="shared" ref="K16:P16" si="5">K14-K15</f>
         <v>42.705999999999968</v>
       </c>
       <c r="L16" s="25">
-        <f>L14-L15</f>
+        <f t="shared" si="5"/>
         <v>110.45600000000002</v>
       </c>
       <c r="M16" s="25">
-        <f>M14-M15</f>
+        <f t="shared" si="5"/>
         <v>49.077999999999946</v>
       </c>
       <c r="N16" s="25">
-        <f>N14-N15</f>
+        <f t="shared" si="5"/>
         <v>67.82600000000015</v>
       </c>
       <c r="O16" s="25">
-        <f>O14-O15</f>
+        <f t="shared" si="5"/>
         <v>-14.846000000000073</v>
+      </c>
+      <c r="P16" s="25">
+        <f t="shared" si="5"/>
+        <v>-14.741999999999983</v>
       </c>
       <c r="V16" s="25">
         <f>V14-V15</f>
@@ -2544,7 +2619,7 @@
         <v>270.06599999999969</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>73</v>
       </c>
@@ -2565,12 +2640,15 @@
         <v>1.845</v>
       </c>
       <c r="N17" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3170000000000002</v>
       </c>
       <c r="O17" s="26">
         <v>1.623</v>
       </c>
+      <c r="P17" s="26">
+        <v>2.0920000000000001</v>
+      </c>
       <c r="V17" s="26">
         <v>5.6020000000000003</v>
       </c>
@@ -2581,7 +2659,7 @@
         <v>7.056</v>
       </c>
     </row>
-    <row r="18" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="3" t="s">
         <v>74</v>
       </c>
@@ -2595,24 +2673,28 @@
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="25">
-        <f>K16-K17</f>
+        <f t="shared" ref="K18:P18" si="6">K16-K17</f>
         <v>41.767999999999965</v>
       </c>
       <c r="L18" s="25">
-        <f>L16-L17</f>
+        <f t="shared" si="6"/>
         <v>108.50000000000001</v>
       </c>
       <c r="M18" s="25">
-        <f>M16-M17</f>
+        <f t="shared" si="6"/>
         <v>47.232999999999947</v>
       </c>
       <c r="N18" s="25">
-        <f>N16-N17</f>
+        <f t="shared" si="6"/>
         <v>65.509000000000157</v>
       </c>
       <c r="O18" s="25">
-        <f>O16-O17</f>
+        <f t="shared" si="6"/>
         <v>-16.469000000000072</v>
+      </c>
+      <c r="P18" s="25">
+        <f t="shared" si="6"/>
+        <v>-16.833999999999982</v>
       </c>
       <c r="V18" s="25">
         <f>V16-V17</f>
@@ -2627,7 +2709,7 @@
         <v>263.00999999999971</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
@@ -2641,24 +2723,28 @@
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24">
-        <f>K18/K20</f>
+        <f t="shared" ref="K19:P19" si="7">K18/K20</f>
         <v>0.66957358127604938</v>
       </c>
       <c r="L19" s="24">
-        <f>L18/L20</f>
+        <f t="shared" si="7"/>
         <v>1.7662955004232601</v>
       </c>
       <c r="M19" s="24">
-        <f>M18/M20</f>
+        <f t="shared" si="7"/>
         <v>0.80333696169807378</v>
       </c>
       <c r="N19" s="24">
-        <f>N18/N20</f>
+        <f t="shared" si="7"/>
         <v>1.0991996241421573</v>
       </c>
       <c r="O19" s="24">
-        <f>O18/O20</f>
+        <f t="shared" si="7"/>
         <v>-0.31624325517983126</v>
+      </c>
+      <c r="P19" s="46">
+        <f t="shared" si="7"/>
+        <v>-0.33373644455898932</v>
       </c>
       <c r="V19" s="24">
         <f>V18/V20</f>
@@ -2673,7 +2759,7 @@
         <v>4.4131416010872977</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2700,6 +2786,9 @@
       <c r="O20" s="26">
         <v>52.076999999999998</v>
       </c>
+      <c r="P20" s="26">
+        <v>50.441000000000003</v>
+      </c>
       <c r="V20" s="30">
         <v>64.427999999999997</v>
       </c>
@@ -2710,7 +2799,7 @@
         <v>59.597000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
         <v>75</v>
       </c>
@@ -2728,6 +2817,10 @@
         <f>O5/K5-1</f>
         <v>4.0128998406716132E-2</v>
       </c>
+      <c r="P22" s="29">
+        <f t="shared" ref="P22" si="8">P5/L5-1</f>
+        <v>-6.9097531363820353E-2</v>
+      </c>
       <c r="W22" s="29">
         <f>W5/V5-1</f>
         <v>-0.137366539399013</v>
@@ -2737,7 +2830,7 @@
         <v>0.18793978595910144</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>76</v>
       </c>
@@ -2746,20 +2839,24 @@
         <v>0.17373497840556307</v>
       </c>
       <c r="L23" s="43">
-        <f t="shared" ref="L23:M23" si="2">L5/K5-1</f>
+        <f t="shared" ref="L23:M23" si="9">L5/K5-1</f>
         <v>0.10678841317882548</v>
       </c>
       <c r="M23" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>4.6609238596288405E-2</v>
       </c>
       <c r="N23" s="43">
-        <f t="shared" ref="N23:O23" si="3">N5/M5-1</f>
+        <f t="shared" ref="N23:O23" si="10">N5/M5-1</f>
         <v>0.28303614830527235</v>
       </c>
       <c r="O23" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>-0.3001593830644087</v>
+      </c>
+      <c r="P23" s="43">
+        <f t="shared" ref="P23" si="11">P5/O5-1</f>
+        <v>-9.4381873168282171E-3</v>
       </c>
       <c r="V23" s="18" t="s">
         <v>130</v>
@@ -2771,7 +2868,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B24" s="33" t="s">
         <v>106</v>
       </c>
@@ -2790,6 +2887,10 @@
         <f>O3/K3-1</f>
         <v>-3.068208531491301E-2</v>
       </c>
+      <c r="P24" s="27">
+        <f t="shared" ref="P24:P25" si="12">P3/L3-1</f>
+        <v>-0.15073189979066348</v>
+      </c>
       <c r="W24" s="27">
         <f>W3/V3-1</f>
         <v>-0.15017970696506955</v>
@@ -2799,7 +2900,7 @@
         <v>0.17097618828260042</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B25" s="34" t="s">
         <v>105</v>
       </c>
@@ -2818,6 +2919,10 @@
         <f>O4/K4-1</f>
         <v>0.13254099593801705</v>
       </c>
+      <c r="P25" s="27">
+        <f t="shared" si="12"/>
+        <v>5.0775329868395058E-2</v>
+      </c>
       <c r="W25" s="27">
         <f>W4/V4-1</f>
         <v>-0.11848208231966062</v>
@@ -2827,7 +2932,7 @@
         <v>0.21204227615827609</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
@@ -2852,19 +2957,23 @@
         <v>0.63662114985195983</v>
       </c>
       <c r="N27" s="27">
-        <f t="shared" ref="N27" si="4">N7/N5</f>
+        <f t="shared" ref="N27" si="13">N7/N5</f>
         <v>0.58305442014615716</v>
       </c>
       <c r="O27" s="27">
         <f>O7/O5</f>
         <v>0.55310902822720542</v>
       </c>
+      <c r="P27" s="27">
+        <f t="shared" ref="P27" si="14">P7/P5</f>
+        <v>0.57868116771892864</v>
+      </c>
       <c r="V27" s="27">
-        <f t="shared" ref="V27:W27" si="5">V7/V5</f>
+        <f t="shared" ref="V27:W27" si="15">V7/V5</f>
         <v>0.59367227764938779</v>
       </c>
       <c r="W27" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>0.60511124393034577</v>
       </c>
       <c r="X27" s="27">
@@ -2872,7 +2981,7 @@
         <v>0.6227146430910846</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
@@ -2897,19 +3006,23 @@
         <v>8.0351540059215978E-2</v>
       </c>
       <c r="N28" s="27">
-        <f t="shared" ref="N28" si="6">N12/N5</f>
+        <f t="shared" ref="N28" si="16">N12/N5</f>
         <v>8.4498856075629139E-2</v>
       </c>
       <c r="O28" s="27">
         <f>O12/O5</f>
         <v>-1.1966602769322474E-2</v>
       </c>
+      <c r="P28" s="27">
+        <f t="shared" ref="P28" si="17">P12/P5</f>
+        <v>-2.721431490353244E-3</v>
+      </c>
       <c r="V28" s="27">
-        <f t="shared" ref="V28:W28" si="7">V12/V5</f>
+        <f t="shared" ref="V28:W28" si="18">V12/V5</f>
         <v>1.9339383998059276E-2</v>
       </c>
       <c r="W28" s="27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="18"/>
         <v>-6.5492752250603924E-3</v>
       </c>
       <c r="X28" s="27">
@@ -2917,7 +3030,7 @@
         <v>9.2406527959732393E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
@@ -2942,19 +3055,23 @@
         <v>5.4220248353882131E-2</v>
       </c>
       <c r="N29" s="27">
-        <f t="shared" ref="N29" si="8">N16/N5</f>
+        <f t="shared" ref="N29" si="19">N16/N5</f>
         <v>5.8402570105730238E-2</v>
       </c>
       <c r="O29" s="27">
         <f>O16/O5</f>
         <v>-1.8266109882105801E-2</v>
       </c>
+      <c r="P29" s="27">
+        <f t="shared" ref="P29" si="20">P16/P5</f>
+        <v>-1.8310973542121304E-2</v>
+      </c>
       <c r="V29" s="27">
-        <f t="shared" ref="V29:W29" si="9">V16/V5</f>
+        <f t="shared" ref="V29:W29" si="21">V16/V5</f>
         <v>1.2409355262784E-2</v>
       </c>
       <c r="W29" s="27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-3.4860996280777067E-2</v>
       </c>
       <c r="X29" s="27">
@@ -2962,7 +3079,7 @@
         <v>7.2739799524236287E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
@@ -2987,19 +3104,23 @@
         <v>5.218193468558039E-2</v>
       </c>
       <c r="N30" s="27">
-        <f t="shared" ref="N30" si="10">N18/N5</f>
+        <f t="shared" ref="N30" si="22">N18/N5</f>
         <v>5.6407483340552046E-2</v>
       </c>
       <c r="O30" s="27">
         <f>O18/O5</f>
         <v>-2.0263004421958795E-2</v>
       </c>
+      <c r="P30" s="27">
+        <f t="shared" ref="P30" si="23">P18/P5</f>
+        <v>-2.0909437566684987E-2</v>
+      </c>
       <c r="V30" s="27">
-        <f t="shared" ref="V30:W30" si="11">V18/V5</f>
+        <f t="shared" ref="V30:W30" si="24">V18/V5</f>
         <v>1.0863154013181798E-2</v>
       </c>
       <c r="W30" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>-3.6482237062709783E-2</v>
       </c>
       <c r="X30" s="27">
@@ -3007,7 +3128,7 @@
         <v>7.0839330655726326E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
@@ -3032,19 +3153,23 @@
         <v>0.25027115381677661</v>
       </c>
       <c r="N31" s="27">
-        <f t="shared" ref="N31" si="12">N15/N14</f>
+        <f t="shared" ref="N31" si="25">N15/N14</f>
         <v>0.25608177769978241</v>
       </c>
       <c r="O31" s="27">
         <f>O15/O14</f>
         <v>0.12839781600422653</v>
       </c>
+      <c r="P31" s="27">
+        <f t="shared" ref="P31" si="26">P15/P14</f>
+        <v>-0.61857707509881543</v>
+      </c>
       <c r="V31" s="27">
-        <f t="shared" ref="V31:W31" si="13">V15/V14</f>
+        <f t="shared" ref="V31:W31" si="27">V15/V14</f>
         <v>0.27868957661516464</v>
       </c>
       <c r="W31" s="27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="27"/>
         <v>-1.2352748086904748</v>
       </c>
       <c r="X31" s="27">
@@ -3052,12 +3177,12 @@
         <v>0.12592645335853514</v>
       </c>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B33" s="28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B34" s="34" t="s">
         <v>122</v>
       </c>
@@ -3069,12 +3194,16 @@
         <f>352+156</f>
         <v>508</v>
       </c>
+      <c r="P34" s="1">
+        <f>358+155</f>
+        <v>513</v>
+      </c>
       <c r="X34" s="1">
         <f>154+351</f>
         <v>505</v>
       </c>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B35" s="34" t="s">
         <v>123</v>
       </c>
@@ -3086,12 +3215,16 @@
         <f>171+49</f>
         <v>220</v>
       </c>
+      <c r="P35" s="1">
+        <f>172+49</f>
+        <v>221</v>
+      </c>
       <c r="X35" s="1">
         <f>51+173</f>
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>124</v>
       </c>
@@ -3103,23 +3236,30 @@
         <f>O34+O35</f>
         <v>728</v>
       </c>
+      <c r="P36" s="1">
+        <f>P34+P35</f>
+        <v>734</v>
+      </c>
       <c r="X36" s="1">
         <f>X34+X35</f>
         <v>729</v>
       </c>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B38" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B39" s="3" t="s">
         <v>6</v>
       </c>
       <c r="O39" s="25">
         <v>468.37799999999999</v>
       </c>
+      <c r="P39" s="25">
+        <v>369.95600000000002</v>
+      </c>
       <c r="W39" s="25">
         <v>1104.8620000000001</v>
       </c>
@@ -3127,13 +3267,16 @@
         <v>823.13900000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>82</v>
       </c>
       <c r="O40" s="26">
         <v>88.807000000000002</v>
       </c>
+      <c r="P40" s="26">
+        <v>79.72</v>
+      </c>
       <c r="W40" s="26">
         <v>83.856999999999999</v>
       </c>
@@ -3141,13 +3284,16 @@
         <v>69.102000000000004</v>
       </c>
     </row>
-    <row r="41" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
         <v>83</v>
       </c>
       <c r="O41" s="25">
         <v>562.51</v>
       </c>
+      <c r="P41" s="25">
+        <v>708.024</v>
+      </c>
       <c r="W41" s="25">
         <v>404.053</v>
       </c>
@@ -3155,13 +3301,16 @@
         <v>525.86400000000003</v>
       </c>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>84</v>
       </c>
       <c r="O42" s="26">
         <v>93.179000000000002</v>
       </c>
+      <c r="P42" s="26">
+        <v>104.887</v>
+      </c>
       <c r="W42" s="26">
         <v>68.856999999999999</v>
       </c>
@@ -3169,7 +3318,7 @@
         <v>89.653999999999996</v>
       </c>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>85</v>
       </c>
@@ -3178,21 +3327,25 @@
         <v>0</v>
       </c>
       <c r="L43" s="26">
-        <f t="shared" ref="L43:N43" si="14">SUM(L39:L42)</f>
+        <f t="shared" ref="L43:N43" si="28">SUM(L39:L42)</f>
         <v>0</v>
       </c>
       <c r="M43" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="N43" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O43" s="26">
         <f>SUM(O39:O42)</f>
         <v>1212.874</v>
       </c>
+      <c r="P43" s="26">
+        <f>SUM(P39:P42)</f>
+        <v>1262.587</v>
+      </c>
       <c r="W43" s="26">
         <f>SUM(W39:W42)</f>
         <v>1661.6289999999999</v>
@@ -3202,13 +3355,16 @@
         <v>1507.759</v>
       </c>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="O44" s="26">
         <v>497.976</v>
       </c>
+      <c r="P44" s="26">
+        <v>511.18099999999998</v>
+      </c>
       <c r="W44" s="26">
         <v>550.58699999999999</v>
       </c>
@@ -3216,13 +3372,16 @@
         <v>508.33600000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="O45" s="26">
         <v>671.99099999999999</v>
       </c>
+      <c r="P45" s="26">
+        <v>740.62699999999995</v>
+      </c>
       <c r="W45" s="26">
         <v>893.98900000000003</v>
       </c>
@@ -3230,13 +3389,16 @@
         <v>698.23099999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>88</v>
       </c>
       <c r="O46" s="26">
         <v>224.46199999999999</v>
       </c>
+      <c r="P46" s="26">
+        <v>219.59800000000001</v>
+      </c>
       <c r="W46" s="26">
         <v>208.697</v>
       </c>
@@ -3244,7 +3406,7 @@
         <v>225.16499999999999</v>
       </c>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>89</v>
       </c>
@@ -3253,21 +3415,25 @@
         <v>0</v>
       </c>
       <c r="L47" s="26">
-        <f t="shared" ref="L47:N47" si="15">L43+L44+L45+L46</f>
+        <f t="shared" ref="L47:N47" si="29">L43+L44+L45+L46</f>
         <v>0</v>
       </c>
       <c r="M47" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N47" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="O47" s="26">
         <f>O43+O44+O45+O46</f>
         <v>2607.3029999999999</v>
       </c>
+      <c r="P47" s="26">
+        <f>P43+P44+P45+P46</f>
+        <v>2733.9929999999999</v>
+      </c>
       <c r="W47" s="26">
         <f>W43+W44+W45+W46</f>
         <v>3314.902</v>
@@ -3277,18 +3443,21 @@
         <v>2939.491</v>
       </c>
     </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:24" x14ac:dyDescent="0.15">
       <c r="O48" s="26"/>
       <c r="W48" s="26"/>
       <c r="X48" s="26"/>
     </row>
-    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>90</v>
       </c>
       <c r="O49" s="26">
         <v>311.35199999999998</v>
       </c>
+      <c r="P49" s="26">
+        <v>408.29700000000003</v>
+      </c>
       <c r="W49" s="26">
         <v>289.39600000000002</v>
       </c>
@@ -3296,13 +3465,16 @@
         <v>374.82900000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
         <v>91</v>
       </c>
       <c r="O50" s="26">
         <v>320.68099999999998</v>
       </c>
+      <c r="P50" s="26">
+        <v>342.69</v>
+      </c>
       <c r="W50" s="26">
         <v>396.36500000000001</v>
       </c>
@@ -3310,13 +3482,16 @@
         <v>395.815</v>
       </c>
     </row>
-    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>92</v>
       </c>
       <c r="O51" s="26">
         <v>195.59899999999999</v>
       </c>
+      <c r="P51" s="26">
+        <v>202.66900000000001</v>
+      </c>
       <c r="W51" s="26">
         <v>248.846</v>
       </c>
@@ -3324,13 +3499,16 @@
         <v>222.82300000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>93</v>
       </c>
       <c r="O52" s="26">
         <v>25.4</v>
       </c>
+      <c r="P52" s="26">
+        <v>5.5819999999999999</v>
+      </c>
       <c r="W52" s="26">
         <v>24.792000000000002</v>
       </c>
@@ -3338,7 +3516,7 @@
         <v>21.773</v>
       </c>
     </row>
-    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
         <v>94</v>
       </c>
@@ -3347,21 +3525,25 @@
         <v>0</v>
       </c>
       <c r="L53" s="26">
-        <f t="shared" ref="L53:N53" si="16">SUM(L49:L52)</f>
+        <f t="shared" ref="L53:N53" si="30">SUM(L49:L52)</f>
         <v>0</v>
       </c>
       <c r="M53" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="N53" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="O53" s="26">
         <f>SUM(O49:O52)</f>
         <v>853.03199999999981</v>
       </c>
+      <c r="P53" s="26">
+        <f>SUM(P49:P52)</f>
+        <v>959.23800000000006</v>
+      </c>
       <c r="W53" s="26">
         <f>SUM(W49:W52)</f>
         <v>959.399</v>
@@ -3371,13 +3553,16 @@
         <v>1015.24</v>
       </c>
     </row>
-    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
       <c r="O54" s="26">
         <v>662.322</v>
       </c>
+      <c r="P54" s="26">
+        <v>714.26499999999999</v>
+      </c>
       <c r="W54" s="26">
         <v>957.55799999999999</v>
       </c>
@@ -3385,13 +3570,16 @@
         <v>697.26400000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B55" s="3" t="s">
         <v>96</v>
       </c>
       <c r="O55" s="25">
         <v>303.90100000000001</v>
       </c>
+      <c r="P55" s="25">
+        <v>304.21899999999999</v>
+      </c>
       <c r="W55" s="25">
         <v>343.91</v>
       </c>
@@ -3399,13 +3587,16 @@
         <v>303.57400000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>97</v>
       </c>
       <c r="O56" s="26">
         <v>83.242999999999995</v>
       </c>
+      <c r="P56" s="26">
+        <v>83.415000000000006</v>
+      </c>
       <c r="W56" s="26">
         <v>104.693</v>
       </c>
@@ -3413,7 +3604,7 @@
         <v>86.088999999999999</v>
       </c>
     </row>
-    <row r="57" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
         <v>98</v>
       </c>
@@ -3422,21 +3613,25 @@
         <v>0</v>
       </c>
       <c r="L57" s="26">
-        <f t="shared" ref="L57:N57" si="17">L53+L54+L55+L56</f>
+        <f t="shared" ref="L57:N57" si="31">L53+L54+L55+L56</f>
         <v>0</v>
       </c>
       <c r="M57" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N57" s="26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="O57" s="26">
         <f>O53+O54+O55+O56</f>
         <v>1902.4979999999998</v>
       </c>
+      <c r="P57" s="26">
+        <f>P53+P54+P55+P56</f>
+        <v>2061.1370000000002</v>
+      </c>
       <c r="W57" s="26">
         <f>W53+W54+W55+W56</f>
         <v>2365.56</v>
@@ -3446,17 +3641,20 @@
         <v>2102.1669999999999</v>
       </c>
     </row>
-    <row r="58" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:24" x14ac:dyDescent="0.15">
       <c r="W58" s="26"/>
       <c r="X58" s="26"/>
     </row>
-    <row r="59" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>99</v>
       </c>
       <c r="O59" s="26">
         <v>704.80499999999995</v>
       </c>
+      <c r="P59" s="26">
+        <v>672.92700000000002</v>
+      </c>
       <c r="W59" s="26">
         <v>949.31200000000001</v>
       </c>
@@ -3464,7 +3662,7 @@
         <v>837.32399999999996</v>
       </c>
     </row>
-    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>100</v>
       </c>
@@ -3472,6 +3670,10 @@
         <f>O59+O57</f>
         <v>2607.3029999999999</v>
       </c>
+      <c r="P60" s="26">
+        <f>P59+P57</f>
+        <v>2734.0640000000003</v>
+      </c>
       <c r="W60" s="26">
         <f>W59+W57</f>
         <v>3314.8719999999998</v>
@@ -3481,16 +3683,16 @@
         <v>2939.491</v>
       </c>
     </row>
-    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:24" x14ac:dyDescent="0.15">
       <c r="X61" s="26"/>
     </row>
-    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>101</v>
       </c>
       <c r="X62" s="26"/>
     </row>
-    <row r="63" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>102</v>
       </c>
@@ -3498,6 +3700,10 @@
         <f>O47-O57</f>
         <v>704.80500000000006</v>
       </c>
+      <c r="P63" s="26">
+        <f t="shared" ref="P63" si="32">P47-P57</f>
+        <v>672.85599999999977</v>
+      </c>
       <c r="W63" s="26">
         <f>W47-W57</f>
         <v>949.3420000000001</v>
@@ -3507,11 +3713,15 @@
         <v>837.32400000000007</v>
       </c>
     </row>
-    <row r="64" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:24" x14ac:dyDescent="0.15">
       <c r="O64" s="30">
         <f>O63/O20</f>
         <v>13.533901722449452</v>
       </c>
+      <c r="P64" s="30">
+        <f t="shared" ref="P64" si="33">P63/P20</f>
+        <v>13.339465910667904</v>
+      </c>
       <c r="W64" s="26">
         <f>W63/W20</f>
         <v>15.177087496602773</v>
@@ -3521,7 +3731,7 @@
         <v>14.049767605751969</v>
       </c>
     </row>
-    <row r="66" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B66" s="3" t="s">
         <v>132</v>
       </c>
@@ -3530,12 +3740,16 @@
         <v>0.30147282658463137</v>
       </c>
     </row>
-    <row r="67" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B67" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="69" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P67" s="27">
+        <f>P41/O41-1</f>
+        <v>0.25868695667632569</v>
+      </c>
+    </row>
+    <row r="69" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B69" s="3" t="s">
         <v>134</v>
       </c>
@@ -3544,7 +3758,7 @@
         <v>-0.25498478543021663</v>
       </c>
     </row>
-    <row r="70" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>135</v>
       </c>
@@ -3555,11 +3769,12 @@
     <hyperlink ref="X1" r:id="rId2" location="i0673e2349c7140edbe9ed5c39f3f5977_73" xr:uid="{7A703C4E-1B76-4F2D-BB2D-470EDEEB4BF3}"/>
     <hyperlink ref="M1" r:id="rId3" location="id3a4d98ceaf340b49a9b4120a6f6242d_31" xr:uid="{F8710F00-6532-1246-AC65-F36142AF7599}"/>
     <hyperlink ref="L1" r:id="rId4" location="ib223de12289d413dbeacbd98f83fd0f5_16" xr:uid="{CB4C7934-1202-5C47-ADA3-87001AAE1270}"/>
+    <hyperlink ref="P1" r:id="rId5" xr:uid="{1A8AB90C-3113-8A4A-A39C-004613218F30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="N7 N15:N17 N14 N12" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Q322 results for $ANF (need review GAAP/non-GAAP EPS)
</commit_message>
<xml_diff>
--- a/$ANF.xlsx
+++ b/$ANF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89527E70-CB65-47C4-A8FA-C37C4B706101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE8CF1F-8D54-2645-BFF7-2BBE7D56C224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="18900" xr2:uid="{BED0471A-CBC0-4084-A037-CD3E53E820DA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18900" activeTab="1" xr2:uid="{BED0471A-CBC0-4084-A037-CD3E53E820DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="144">
   <si>
     <t>$ANF</t>
   </si>
@@ -446,19 +456,32 @@
   </si>
   <si>
     <t>Ratios</t>
+  </si>
+  <si>
+    <t>Inventory/Revenue</t>
+  </si>
+  <si>
+    <t>P/S</t>
+  </si>
+  <si>
+    <t>EV/S</t>
+  </si>
+  <si>
+    <t>Chairman Terry Burman (since 2018) announces to to step down on Jan 28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="#.#\x"/>
     <numFmt numFmtId="167" formatCode="0.#\x"/>
+    <numFmt numFmtId="170" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,6 +557,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -656,7 +686,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -686,7 +716,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -755,6 +784,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -767,29 +808,22 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -874,16 +908,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -898,8 +932,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12430125" y="6350"/>
-          <a:ext cx="0" cy="12760325"/>
+          <a:off x="13128625" y="0"/>
+          <a:ext cx="0" cy="15240000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -932,8 +966,8 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -948,8 +982,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15135225" y="0"/>
-          <a:ext cx="0" cy="11191875"/>
+          <a:off x="18027650" y="0"/>
+          <a:ext cx="0" cy="15252700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1274,71 +1308,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC0834B-0A87-42F0-A33F-D4A328ED8962}">
   <dimension ref="B2:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="47" t="s">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="H5" s="47" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="H5" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="49"/>
-      <c r="S5" s="47" t="s">
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="48"/>
+      <c r="S5" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="49"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="48"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8">
-        <v>18.78</v>
+        <v>22.62</v>
       </c>
       <c r="D6" s="14"/>
-      <c r="H6" s="41">
-        <v>44743</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>125</v>
-      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="9"/>
-      <c r="S6" s="37" t="s">
+      <c r="S6" s="36" t="s">
         <v>108</v>
       </c>
       <c r="T6" s="8"/>
@@ -1346,27 +1376,31 @@
       <c r="V6" s="8"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="16">
-        <f>'Financial Model'!P20</f>
-        <v>50.441000000000003</v>
+        <f>'Financial Model'!Q20</f>
+        <v>49.485999999999997</v>
       </c>
       <c r="D7" s="14" t="str">
         <f>$C$27</f>
-        <v>Q222</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="8"/>
+        <v>Q322</v>
+      </c>
+      <c r="H7" s="40">
+        <v>44866</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="9"/>
-      <c r="S7" s="39" t="s">
+      <c r="S7" s="38" t="s">
         <v>113</v>
       </c>
       <c r="T7" s="8"/>
@@ -1374,56 +1408,50 @@
       <c r="V7" s="8"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="62">
         <f>C6*C7</f>
-        <v>947.28198000000009</v>
+        <v>1119.3733199999999</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="H8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>126</v>
-      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="9"/>
-      <c r="S8" s="37"/>
+      <c r="S8" s="36"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16">
-        <f>'Financial Model'!P39</f>
-        <v>369.95600000000002</v>
+      <c r="C9" s="62">
+        <f>'Financial Model'!Q39</f>
+        <v>257.33199999999999</v>
       </c>
       <c r="D9" s="14" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$27</f>
-        <v>Q222</v>
+        <v>Q322</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="42" t="s">
-        <v>127</v>
-      </c>
+      <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="9"/>
-      <c r="S9" s="37" t="s">
+      <c r="S9" s="36" t="s">
         <v>109</v>
       </c>
       <c r="T9" s="8"/>
@@ -1431,29 +1459,27 @@
       <c r="V9" s="8"/>
       <c r="W9" s="9"/>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16">
-        <f>'Financial Model'!P55</f>
-        <v>304.21899999999999</v>
+      <c r="C10" s="62">
+        <f>'Financial Model'!Q40</f>
+        <v>108.468</v>
       </c>
       <c r="D10" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>Q222</v>
+        <v>Q322</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="42" t="s">
-        <v>128</v>
-      </c>
+      <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="9"/>
-      <c r="S10" s="39" t="s">
+      <c r="S10" s="38" t="s">
         <v>114</v>
       </c>
       <c r="T10" s="8"/>
@@ -1461,52 +1487,54 @@
       <c r="V10" s="8"/>
       <c r="W10" s="9"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="62">
         <f>C9-C10</f>
-        <v>65.737000000000023</v>
+        <v>148.86399999999998</v>
       </c>
       <c r="D11" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>Q222</v>
+        <v>Q322</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="42" t="s">
-        <v>129</v>
-      </c>
+      <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
-      <c r="S11" s="35"/>
+      <c r="S11" s="34"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="9"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="63">
         <f>C8-C11</f>
-        <v>881.54498000000012</v>
+        <v>970.50931999999989</v>
       </c>
       <c r="D12" s="15"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8"/>
+      <c r="H12" s="40">
+        <v>44743</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
-      <c r="S12" s="37" t="s">
+      <c r="S12" s="36" t="s">
         <v>110</v>
       </c>
       <c r="T12" s="8"/>
@@ -1514,7 +1542,7 @@
       <c r="V12" s="8"/>
       <c r="W12" s="9"/>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.15">
       <c r="H13" s="6"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -1523,7 +1551,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="9"/>
-      <c r="S13" s="39" t="s">
+      <c r="S13" s="38" t="s">
         <v>115</v>
       </c>
       <c r="T13" s="8"/>
@@ -1531,12 +1559,12 @@
       <c r="V13" s="8"/>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="H14" s="41">
-        <v>44136</v>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="H14" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -1544,21 +1572,21 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="9"/>
-      <c r="S14" s="35"/>
+      <c r="S14" s="34"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="47" t="s">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B15" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="42" t="s">
-        <v>138</v>
+      <c r="I15" s="41" t="s">
+        <v>127</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -1566,7 +1594,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
-      <c r="S15" s="37" t="s">
+      <c r="S15" s="36" t="s">
         <v>111</v>
       </c>
       <c r="T15" s="8"/>
@@ -1574,23 +1602,25 @@
       <c r="V15" s="8"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="52"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="8"/>
+      <c r="I16" s="41" t="s">
+        <v>128</v>
+      </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
-      <c r="S16" s="39" t="s">
+      <c r="S16" s="38" t="s">
         <v>116</v>
       </c>
       <c r="T16" s="8"/>
@@ -1598,23 +1628,25 @@
       <c r="V16" s="8"/>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="52"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="8"/>
+      <c r="I17" s="41" t="s">
+        <v>129</v>
+      </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="9"/>
-      <c r="S17" s="40" t="s">
+      <c r="S17" s="39" t="s">
         <v>117</v>
       </c>
       <c r="T17" s="8"/>
@@ -1622,14 +1654,14 @@
       <c r="V17" s="8"/>
       <c r="W17" s="9"/>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="52"/>
       <c r="H18" s="6"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1638,7 +1670,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="9"/>
-      <c r="S18" s="38" t="s">
+      <c r="S18" s="37" t="s">
         <v>112</v>
       </c>
       <c r="T18" s="8"/>
@@ -1646,10 +1678,10 @@
       <c r="V18" s="8"/>
       <c r="W18" s="9"/>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B19" s="13"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
       <c r="H19" s="6"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1658,7 +1690,7 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="9"/>
-      <c r="S19" s="40" t="s">
+      <c r="S19" s="39" t="s">
         <v>118</v>
       </c>
       <c r="T19" s="8"/>
@@ -1666,166 +1698,191 @@
       <c r="V19" s="8"/>
       <c r="W19" s="9"/>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="H20" s="7"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="11"/>
-      <c r="S20" s="36"/>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="H20" s="40">
+        <v>44136</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="9"/>
+      <c r="S20" s="35"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
       <c r="W20" s="11"/>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B22" s="47" t="s">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="H21" s="6"/>
+      <c r="I21" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B22" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="55"/>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="D23" s="52"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="11"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="51">
         <v>1892</v>
       </c>
-      <c r="D24" s="55"/>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="D24" s="52"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B25" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="54">
-        <f>'Financial Model'!P36</f>
-        <v>734</v>
-      </c>
-      <c r="D25" s="55"/>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C25" s="51">
+        <f>'Financial Model'!Q36</f>
+        <v>751</v>
+      </c>
+      <c r="D25" s="52"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B26" s="6"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="45">
-        <v>44798</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C27" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="44">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="59"/>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B31" s="47" t="s">
+      <c r="D28" s="50"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="B31" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="49"/>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C31" s="47"/>
+      <c r="D31" s="48"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="56">
+      <c r="C32" s="57">
         <f>C6/'Financial Model'!O18</f>
-        <v>-1.1403242455522447</v>
-      </c>
-      <c r="D32" s="57"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+        <v>-1.3734895864958347</v>
+      </c>
+      <c r="D32" s="58"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="50">
-        <f>C6/'Financial Model'!O19</f>
-        <v>-59.384665735624246</v>
-      </c>
-      <c r="D33" s="51"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="53">
+        <f>C6/SUM('Financial Model'!N19:Q19)</f>
+        <v>55.92365534541274</v>
+      </c>
+      <c r="D33" s="54"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="55"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="51"/>
+      <c r="D34" s="52"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="50">
-        <f>C6/'Financial Model'!P64</f>
-        <v>1.4078524676899669</v>
-      </c>
-      <c r="D35" s="51"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="53">
+        <f>C6/'Financial Model'!Q64</f>
+        <v>1.7061927095638381</v>
+      </c>
+      <c r="D35" s="54"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="6"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="51"/>
+      <c r="D36" s="52"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="50">
+      <c r="C37" s="53">
         <f>C6/'Financial Model'!X19</f>
-        <v>4.2554718831983633</v>
-      </c>
-      <c r="D37" s="51"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+        <v>5.1256003193794974</v>
+      </c>
+      <c r="D37" s="54"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="50">
+      <c r="C38" s="53">
         <f>C12/'Financial Model'!X18</f>
-        <v>3.3517546100908753</v>
-      </c>
-      <c r="D38" s="51"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+        <v>3.6900092011710619</v>
+      </c>
+      <c r="D38" s="54"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
     <mergeCell ref="S5:W5"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
@@ -1842,6 +1899,13 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28:D28" r:id="rId1" display="Link" xr:uid="{D85FB78D-8AAC-49F6-8EB8-C86ABC1A5D8F}"/>
@@ -1854,485 +1918,513 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E83BA2F8-86D4-4ED0-814B-223EC5B59DE2}">
-  <dimension ref="B1:AI70"/>
+  <dimension ref="A1:AI85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P19" sqref="P19"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23:S36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="19" t="s">
+    <row r="1" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="U1" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="V1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="W1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="X1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="Z1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AA1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AB1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AC1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AD1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AE1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AF1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AG1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AH1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="2:35" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="20"/>
-      <c r="H2" s="23">
+    <row r="2" spans="2:35" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="19"/>
+      <c r="H2" s="22">
         <v>44044</v>
       </c>
-      <c r="I2" s="23">
+      <c r="I2" s="22">
         <v>44135</v>
       </c>
-      <c r="K2" s="23">
+      <c r="K2" s="22">
         <v>44682</v>
       </c>
-      <c r="L2" s="23">
+      <c r="L2" s="22">
         <v>44408</v>
       </c>
-      <c r="M2" s="23">
+      <c r="M2" s="22">
         <v>44499</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N2" s="22">
         <v>44590</v>
       </c>
-      <c r="O2" s="23">
+      <c r="O2" s="22">
         <v>44681</v>
       </c>
-      <c r="P2" s="23">
+      <c r="P2" s="22">
         <v>44742</v>
       </c>
-      <c r="V2" s="23">
+      <c r="Q2" s="22">
+        <v>44863</v>
+      </c>
+      <c r="V2" s="22">
         <v>43862</v>
       </c>
-      <c r="W2" s="23">
+      <c r="W2" s="22">
         <v>44226</v>
       </c>
-      <c r="X2" s="23">
+      <c r="X2" s="22">
         <v>44590</v>
       </c>
     </row>
-    <row r="3" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:35" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="32">
+      <c r="H3" s="31">
         <v>429.24799999999999</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="31">
         <v>476.66500000000002</v>
       </c>
-      <c r="K3" s="32">
+      <c r="K3" s="31">
         <v>442.40800000000002</v>
       </c>
-      <c r="L3" s="32">
+      <c r="L3" s="31">
         <v>514.48299999999995</v>
       </c>
-      <c r="M3" s="32">
+      <c r="M3" s="31">
         <v>522.31100000000004</v>
       </c>
-      <c r="N3" s="32">
+      <c r="N3" s="31">
         <f>X3-M3-L3-K3</f>
         <v>668.7769999999997</v>
       </c>
-      <c r="O3" s="32">
+      <c r="O3" s="31">
         <v>428.834</v>
       </c>
-      <c r="P3" s="32">
+      <c r="P3" s="31">
         <v>436.93400000000003</v>
       </c>
-      <c r="V3" s="32">
+      <c r="Q3" s="31">
+        <v>457.75200000000001</v>
+      </c>
+      <c r="V3" s="31">
         <v>2158.5140000000001</v>
       </c>
-      <c r="W3" s="32">
+      <c r="W3" s="31">
         <v>1834.3489999999999</v>
       </c>
-      <c r="X3" s="32">
+      <c r="X3" s="31">
         <v>2147.9789999999998</v>
       </c>
     </row>
-    <row r="4" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="2:35" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="31">
         <v>269.08</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="31">
         <v>342.988</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="31">
         <v>338.99700000000001</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="31">
         <v>350.36700000000002</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="31">
         <v>382.84899999999999</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="31">
         <f>X4-M4-L4-K4</f>
         <v>492.57600000000008</v>
       </c>
-      <c r="O4" s="32">
+      <c r="O4" s="31">
         <v>383.928</v>
       </c>
-      <c r="P4" s="32">
+      <c r="P4" s="31">
         <v>368.15699999999998</v>
       </c>
-      <c r="V4" s="32">
+      <c r="Q4" s="31">
+        <v>422.33199999999999</v>
+      </c>
+      <c r="V4" s="31">
         <v>1464.559</v>
       </c>
-      <c r="W4" s="32">
+      <c r="W4" s="31">
         <v>1291.0350000000001</v>
       </c>
-      <c r="X4" s="32">
+      <c r="X4" s="31">
         <v>1564.789</v>
       </c>
     </row>
-    <row r="5" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="24">
         <v>698.32799999999997</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="24">
         <v>819.65200000000004</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25">
+      <c r="J5" s="24"/>
+      <c r="K5" s="24">
         <v>781.40499999999997</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="24">
         <v>864.85</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="24">
         <v>905.16</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="24">
         <f>X5-M5-L5-K5</f>
         <v>1161.3530000000003</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="24">
         <v>812.76199999999994</v>
       </c>
-      <c r="P5" s="25">
+      <c r="P5" s="24">
         <v>805.09100000000001</v>
       </c>
-      <c r="V5" s="25">
+      <c r="Q5" s="24">
+        <v>880.08399999999995</v>
+      </c>
+      <c r="V5" s="24">
         <f>V3+V4</f>
         <v>3623.0730000000003</v>
       </c>
-      <c r="W5" s="25">
+      <c r="W5" s="24">
         <f t="shared" ref="W5:X5" si="0">W3+W4</f>
         <v>3125.384</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5" s="24">
         <f t="shared" si="0"/>
         <v>3712.768</v>
       </c>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H6" s="1">
         <v>274.72000000000003</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <v>295.22000000000003</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26">
+      <c r="J6" s="25"/>
+      <c r="K6" s="25">
         <v>286.27100000000002</v>
       </c>
       <c r="L6" s="1">
         <v>301.36500000000001</v>
       </c>
-      <c r="M6" s="26">
+      <c r="M6" s="25">
         <v>328.916</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="25">
         <f>X6-M6-L6-K6</f>
         <v>484.22099999999995</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="25">
         <v>363.21600000000001</v>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="25">
         <v>339.2</v>
       </c>
-      <c r="V6" s="26">
+      <c r="Q6" s="25">
+        <v>359.26799999999997</v>
+      </c>
+      <c r="V6" s="25">
         <v>1472.155</v>
       </c>
-      <c r="W6" s="26">
+      <c r="W6" s="25">
         <v>1234.1790000000001</v>
       </c>
-      <c r="X6" s="26">
+      <c r="X6" s="25">
         <v>1400.7729999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="24">
         <f>H5-H6</f>
         <v>423.60799999999995</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="24">
         <f>I5-I6</f>
         <v>524.43200000000002</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25">
-        <f t="shared" ref="K7:P7" si="1">K5-K6</f>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24">
+        <f t="shared" ref="K7:Q7" si="1">K5-K6</f>
         <v>495.13399999999996</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="24">
         <f t="shared" si="1"/>
         <v>563.48500000000001</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="24">
         <f t="shared" si="1"/>
         <v>576.24399999999991</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="24">
         <f t="shared" si="1"/>
         <v>677.13200000000029</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="24">
         <f t="shared" si="1"/>
         <v>449.54599999999994</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="24">
         <f t="shared" si="1"/>
         <v>465.89100000000002</v>
       </c>
-      <c r="V7" s="25">
+      <c r="Q7" s="24">
+        <f t="shared" si="1"/>
+        <v>520.81600000000003</v>
+      </c>
+      <c r="V7" s="24">
         <f>V5-V6</f>
         <v>2150.9180000000006</v>
       </c>
-      <c r="W7" s="25">
+      <c r="W7" s="24">
         <f>W5-W6</f>
         <v>1891.2049999999999</v>
       </c>
-      <c r="X7" s="25">
+      <c r="X7" s="24">
         <f>X5-X6</f>
         <v>2311.9949999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
       <c r="H8" s="1">
         <v>310.37</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="25">
         <v>346.26299999999998</v>
       </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26">
+      <c r="J8" s="25"/>
+      <c r="K8" s="25">
         <v>315.50799999999998</v>
       </c>
       <c r="L8" s="1">
         <v>325.935</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="25">
         <v>351.80399999999997</v>
       </c>
-      <c r="N8" s="26">
+      <c r="N8" s="25">
         <f t="shared" ref="N8:N17" si="2">X8-M8-L8-K8</f>
         <v>436.2290000000001</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="25">
         <v>337.54300000000001</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="25">
         <v>340.791</v>
       </c>
-      <c r="V8" s="26">
+      <c r="Q8" s="25">
+        <v>367.33300000000003</v>
+      </c>
+      <c r="V8" s="25">
         <v>1551.2429999999999</v>
       </c>
-      <c r="W8" s="26">
+      <c r="W8" s="25">
         <v>1391.5840000000001</v>
       </c>
-      <c r="X8" s="26">
+      <c r="X8" s="25">
         <v>1429.4760000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
       <c r="H9" s="1">
         <v>97.251999999999995</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="25">
         <v>121</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26">
+      <c r="J9" s="25"/>
+      <c r="K9" s="25">
         <v>120.947</v>
       </c>
       <c r="L9" s="1">
         <v>123.913</v>
       </c>
-      <c r="M9" s="26">
+      <c r="M9" s="25">
         <v>146.26900000000001</v>
       </c>
-      <c r="N9" s="26">
+      <c r="N9" s="25">
         <f t="shared" si="2"/>
         <v>145.68600000000004</v>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="25">
         <v>122.149</v>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="25">
         <v>124.16800000000001</v>
       </c>
-      <c r="V9" s="26">
+      <c r="Q9" s="25">
+        <v>133.20099999999999</v>
+      </c>
+      <c r="V9" s="25">
         <v>464.61500000000001</v>
       </c>
-      <c r="W9" s="26">
+      <c r="W9" s="25">
         <v>463.84300000000002</v>
       </c>
-      <c r="X9" s="26">
+      <c r="X9" s="25">
         <v>536.81500000000005</v>
       </c>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H10" s="1">
         <v>8.0830000000000002</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="25">
         <v>6.3289999999999997</v>
       </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26">
+      <c r="J10" s="25"/>
+      <c r="K10" s="25">
         <v>2.6640000000000001</v>
       </c>
       <c r="L10" s="1">
         <v>0.78600000000000003</v>
       </c>
-      <c r="M10" s="26">
+      <c r="M10" s="25">
         <v>6.7489999999999997</v>
       </c>
-      <c r="N10" s="26">
+      <c r="N10" s="25">
         <f t="shared" si="2"/>
         <v>1.9009999999999994</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="25">
         <v>3.4220000000000002</v>
       </c>
-      <c r="P10" s="26">
+      <c r="P10" s="25">
         <v>2.17</v>
       </c>
-      <c r="V10" s="26">
+      <c r="Q10" s="25">
+        <v>3.7440000000000002</v>
+      </c>
+      <c r="V10" s="25">
         <v>19.135000000000002</v>
       </c>
-      <c r="W10" s="26">
+      <c r="W10" s="25">
         <v>72.936999999999998</v>
       </c>
-      <c r="X10" s="26">
+      <c r="X10" s="25">
         <v>12.1</v>
       </c>
     </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
@@ -2340,840 +2432,911 @@
         <f>-2.356+-3.884</f>
         <v>-6.24</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="25">
         <f>-8.063+0.288</f>
         <v>-7.7750000000000004</v>
       </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26">
+      <c r="J11" s="25"/>
+      <c r="K11" s="25">
         <v>-1.4179999999999999</v>
       </c>
       <c r="L11" s="1">
         <f>-0.088+-1.848</f>
         <v>-1.9360000000000002</v>
       </c>
-      <c r="M11" s="26">
+      <c r="M11" s="25">
         <f>-1.32+0.011</f>
         <v>-1.3090000000000002</v>
       </c>
-      <c r="N11" s="26">
+      <c r="N11" s="25">
         <f t="shared" si="2"/>
         <v>-4.8169999999999993</v>
       </c>
-      <c r="O11" s="26">
+      <c r="O11" s="25">
         <v>-3.8420000000000001</v>
       </c>
-      <c r="P11" s="26">
+      <c r="P11" s="25">
         <v>0.95299999999999996</v>
       </c>
-      <c r="V11" s="26">
+      <c r="Q11" s="25">
+        <v>-1.0049999999999999</v>
+      </c>
+      <c r="V11" s="25">
         <f>47.257-1.4</f>
         <v>45.856999999999999</v>
       </c>
-      <c r="W11" s="26">
+      <c r="W11" s="25">
         <f>-11.636+-5.054</f>
         <v>-16.689999999999998</v>
       </c>
-      <c r="X11" s="26">
+      <c r="X11" s="25">
         <f>-8.327+-1.153</f>
         <v>-9.48</v>
       </c>
     </row>
-    <row r="12" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="24">
         <f>H7-H8-H9-H10-H11</f>
         <v>14.142999999999947</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="24">
         <f>I7-I8-I9-I10-I11</f>
         <v>58.615000000000038</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25">
-        <f t="shared" ref="K12:P12" si="3">K7-K8-K9-K10-K11</f>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24">
+        <f t="shared" ref="K12:Q12" si="3">K7-K8-K9-K10-K11</f>
         <v>57.432999999999971</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="24">
         <f t="shared" si="3"/>
         <v>114.78700000000002</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="24">
         <f t="shared" si="3"/>
         <v>72.730999999999938</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="24">
         <f t="shared" si="3"/>
         <v>98.133000000000152</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="24">
         <f t="shared" si="3"/>
         <v>-9.7260000000000719</v>
       </c>
-      <c r="P12" s="25">
+      <c r="P12" s="24">
         <f t="shared" si="3"/>
         <v>-2.1909999999999834</v>
       </c>
-      <c r="V12" s="25">
+      <c r="Q12" s="24">
+        <f t="shared" si="3"/>
+        <v>17.54300000000001</v>
+      </c>
+      <c r="V12" s="24">
         <f>V7-V8-V9-V10-V11</f>
         <v>70.068000000000623</v>
       </c>
-      <c r="W12" s="25">
+      <c r="W12" s="24">
         <f>W7-W8-W9-W10-W11</f>
         <v>-20.46900000000015</v>
       </c>
-      <c r="X12" s="25">
+      <c r="X12" s="24">
         <f>X7-X8-X9-X10-X11</f>
         <v>343.08399999999972</v>
       </c>
     </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H13" s="1">
         <v>7.0979999999999999</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="25">
         <v>8.8079999999999998</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26">
+      <c r="J13" s="25"/>
+      <c r="K13" s="25">
         <v>8.6059999999999999</v>
       </c>
       <c r="L13" s="1">
         <v>11.275</v>
       </c>
-      <c r="M13" s="26">
+      <c r="M13" s="25">
         <v>7.27</v>
       </c>
-      <c r="N13" s="26">
+      <c r="N13" s="25">
         <f t="shared" si="2"/>
         <v>6.9589999999999996</v>
       </c>
-      <c r="O13" s="26">
+      <c r="O13" s="25">
         <v>7.3070000000000004</v>
       </c>
-      <c r="P13" s="26">
+      <c r="P13" s="25">
         <v>6.9169999999999998</v>
       </c>
-      <c r="V13" s="26">
+      <c r="Q13" s="25">
+        <v>7.2949999999999999</v>
+      </c>
+      <c r="V13" s="25">
         <v>7.7370000000000001</v>
       </c>
-      <c r="W13" s="26">
+      <c r="W13" s="25">
         <v>28.274000000000001</v>
       </c>
-      <c r="X13" s="26">
+      <c r="X13" s="25">
         <v>34.11</v>
       </c>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="25">
         <f>H12-H13</f>
         <v>7.0449999999999475</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f>I12-I13</f>
         <v>49.807000000000038</v>
       </c>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26">
-        <f t="shared" ref="K14:P14" si="4">K12-K13</f>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25">
+        <f t="shared" ref="K14:Q14" si="4">K12-K13</f>
         <v>48.82699999999997</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="25">
         <f t="shared" si="4"/>
         <v>103.51200000000001</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="25">
         <f t="shared" si="4"/>
         <v>65.460999999999942</v>
       </c>
-      <c r="N14" s="26">
+      <c r="N14" s="25">
         <f t="shared" si="4"/>
         <v>91.174000000000149</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="25">
         <f t="shared" si="4"/>
         <v>-17.033000000000072</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="25">
         <f t="shared" si="4"/>
         <v>-9.1079999999999828</v>
       </c>
-      <c r="V14" s="26">
+      <c r="Q14" s="25">
+        <f t="shared" si="4"/>
+        <v>10.24800000000001</v>
+      </c>
+      <c r="V14" s="25">
         <f>V12-V13</f>
         <v>62.331000000000621</v>
       </c>
-      <c r="W14" s="26">
+      <c r="W14" s="25">
         <f>W12-W13</f>
         <v>-48.743000000000151</v>
       </c>
-      <c r="X14" s="26">
+      <c r="X14" s="25">
         <f>X12-X13</f>
         <v>308.97399999999971</v>
       </c>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
       <c r="H15" s="1">
         <v>1.2529999999999999</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="25">
         <v>5.7789999999999999</v>
       </c>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26">
+      <c r="J15" s="25"/>
+      <c r="K15" s="25">
         <v>6.1210000000000004</v>
       </c>
       <c r="L15" s="1">
         <v>-6.944</v>
       </c>
-      <c r="M15" s="26">
+      <c r="M15" s="25">
         <v>16.382999999999999</v>
       </c>
-      <c r="N15" s="26">
+      <c r="N15" s="25">
         <f t="shared" si="2"/>
         <v>23.347999999999999</v>
       </c>
-      <c r="O15" s="26">
+      <c r="O15" s="25">
         <v>-2.1869999999999998</v>
       </c>
-      <c r="P15" s="26">
+      <c r="P15" s="25">
         <v>5.6340000000000003</v>
       </c>
-      <c r="V15" s="26">
+      <c r="Q15" s="25">
+        <v>10.965999999999999</v>
+      </c>
+      <c r="V15" s="25">
         <v>17.370999999999999</v>
       </c>
-      <c r="W15" s="26">
+      <c r="W15" s="25">
         <v>60.210999999999999</v>
       </c>
-      <c r="X15" s="26">
+      <c r="X15" s="25">
         <v>38.908000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="24">
         <f>H14-H15</f>
         <v>5.7919999999999474</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="24">
         <f>I14-I15</f>
         <v>44.028000000000034</v>
       </c>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25">
-        <f t="shared" ref="K16:P16" si="5">K14-K15</f>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24">
+        <f t="shared" ref="K16:Q16" si="5">K14-K15</f>
         <v>42.705999999999968</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="24">
         <f t="shared" si="5"/>
         <v>110.45600000000002</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="24">
         <f t="shared" si="5"/>
         <v>49.077999999999946</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="24">
         <f t="shared" si="5"/>
         <v>67.82600000000015</v>
       </c>
-      <c r="O16" s="25">
+      <c r="O16" s="24">
         <f t="shared" si="5"/>
         <v>-14.846000000000073</v>
       </c>
-      <c r="P16" s="25">
+      <c r="P16" s="24">
         <f t="shared" si="5"/>
         <v>-14.741999999999983</v>
       </c>
-      <c r="V16" s="25">
+      <c r="Q16" s="24">
+        <f t="shared" si="5"/>
+        <v>-0.71799999999998931</v>
+      </c>
+      <c r="V16" s="24">
         <f>V14-V15</f>
         <v>44.960000000000619</v>
       </c>
-      <c r="W16" s="25">
+      <c r="W16" s="24">
         <f>W14-W15</f>
         <v>-108.95400000000015</v>
       </c>
-      <c r="X16" s="25">
+      <c r="X16" s="24">
         <f>X14-X15</f>
         <v>270.06599999999969</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>73</v>
       </c>
       <c r="H17" s="1">
         <v>0.32800000000000001</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="25">
         <v>1.758</v>
       </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26">
+      <c r="J17" s="25"/>
+      <c r="K17" s="25">
         <v>0.93799999999999994</v>
       </c>
       <c r="L17" s="1">
         <v>1.956</v>
       </c>
-      <c r="M17" s="26">
+      <c r="M17" s="25">
         <v>1.845</v>
       </c>
-      <c r="N17" s="26">
+      <c r="N17" s="25">
         <f t="shared" si="2"/>
         <v>2.3170000000000002</v>
       </c>
-      <c r="O17" s="26">
+      <c r="O17" s="25">
         <v>1.623</v>
       </c>
-      <c r="P17" s="26">
+      <c r="P17" s="25">
         <v>2.0920000000000001</v>
       </c>
-      <c r="V17" s="26">
+      <c r="Q17" s="25">
+        <v>1.496</v>
+      </c>
+      <c r="V17" s="25">
         <v>5.6020000000000003</v>
       </c>
-      <c r="W17" s="26">
+      <c r="W17" s="25">
         <v>5.0670000000000002</v>
       </c>
-      <c r="X17" s="26">
+      <c r="X17" s="25">
         <v>7.056</v>
       </c>
     </row>
-    <row r="18" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="24">
         <f>H16-H17</f>
         <v>5.4639999999999471</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="24">
         <f>I16-I17</f>
         <v>42.270000000000032</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25">
-        <f t="shared" ref="K18:P18" si="6">K16-K17</f>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24">
+        <f t="shared" ref="K18:Q18" si="6">K16-K17</f>
         <v>41.767999999999965</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="24">
         <f t="shared" si="6"/>
         <v>108.50000000000001</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="24">
         <f t="shared" si="6"/>
         <v>47.232999999999947</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="24">
         <f t="shared" si="6"/>
         <v>65.509000000000157</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18" s="24">
         <f t="shared" si="6"/>
         <v>-16.469000000000072</v>
       </c>
-      <c r="P18" s="25">
+      <c r="P18" s="24">
         <f t="shared" si="6"/>
         <v>-16.833999999999982</v>
       </c>
-      <c r="V18" s="25">
+      <c r="Q18" s="24">
+        <f t="shared" si="6"/>
+        <v>-2.2139999999999893</v>
+      </c>
+      <c r="V18" s="24">
         <f>V16-V17</f>
         <v>39.358000000000615</v>
       </c>
-      <c r="W18" s="25">
+      <c r="W18" s="24">
         <f>W16-W17</f>
         <v>-114.02100000000016</v>
       </c>
-      <c r="X18" s="25">
+      <c r="X18" s="24">
         <f>X16-X17</f>
         <v>263.00999999999971</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="23">
         <f>H18/H20</f>
         <v>8.7386249140370506E-2</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="23">
         <f>I18/I20</f>
         <v>0.67569295693596398</v>
       </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24">
-        <f t="shared" ref="K19:P19" si="7">K18/K20</f>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23">
+        <f t="shared" ref="K19:Q19" si="7">K18/K20</f>
         <v>0.66957358127604938</v>
       </c>
-      <c r="L19" s="24">
+      <c r="L19" s="23">
         <f t="shared" si="7"/>
         <v>1.7662955004232601</v>
       </c>
-      <c r="M19" s="24">
+      <c r="M19" s="23">
         <f t="shared" si="7"/>
         <v>0.80333696169807378</v>
       </c>
-      <c r="N19" s="24">
+      <c r="N19" s="23">
         <f t="shared" si="7"/>
         <v>1.0991996241421573</v>
       </c>
-      <c r="O19" s="24">
+      <c r="O19" s="23">
         <f t="shared" si="7"/>
         <v>-0.31624325517983126</v>
       </c>
-      <c r="P19" s="46">
+      <c r="P19" s="45">
         <f t="shared" si="7"/>
         <v>-0.33373644455898932</v>
       </c>
-      <c r="V19" s="24">
+      <c r="Q19" s="45">
+        <f t="shared" si="7"/>
+        <v>-4.473992644384249E-2</v>
+      </c>
+      <c r="V19" s="23">
         <f>V18/V20</f>
         <v>0.61088346681567973</v>
       </c>
-      <c r="W19" s="24">
+      <c r="W19" s="23">
         <f>W18/W20</f>
         <v>-1.8228485555786502</v>
       </c>
-      <c r="X19" s="24">
+      <c r="X19" s="23">
         <f>X18/X20</f>
         <v>4.4131416010872977</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="29">
         <v>62.527000000000001</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="29">
         <v>62.558</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30">
+      <c r="J20" s="29"/>
+      <c r="K20" s="29">
         <v>62.38</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L20" s="29">
         <v>61.427999999999997</v>
       </c>
-      <c r="M20" s="30">
+      <c r="M20" s="29">
         <v>58.795999999999999</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="29">
         <f>X20</f>
         <v>59.597000000000001</v>
       </c>
-      <c r="O20" s="26">
+      <c r="O20" s="25">
         <v>52.076999999999998</v>
       </c>
-      <c r="P20" s="26">
+      <c r="P20" s="25">
         <v>50.441000000000003</v>
       </c>
-      <c r="V20" s="30">
+      <c r="Q20" s="25">
+        <v>49.485999999999997</v>
+      </c>
+      <c r="V20" s="29">
         <v>64.427999999999997</v>
       </c>
-      <c r="W20" s="30">
+      <c r="W20" s="29">
         <v>62.551000000000002</v>
       </c>
-      <c r="X20" s="30">
+      <c r="X20" s="29">
         <v>59.597000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29">
+      <c r="K22" s="28"/>
+      <c r="L22" s="28">
         <f>L5/H5-1</f>
         <v>0.23845814574240198</v>
       </c>
-      <c r="M22" s="29">
+      <c r="M22" s="28">
         <f>M5/I5-1</f>
         <v>0.10432232215623216</v>
       </c>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29">
+      <c r="N22" s="28"/>
+      <c r="O22" s="28">
         <f>O5/K5-1</f>
         <v>4.0128998406716132E-2</v>
       </c>
-      <c r="P22" s="29">
+      <c r="P22" s="28">
         <f t="shared" ref="P22" si="8">P5/L5-1</f>
         <v>-6.9097531363820353E-2</v>
       </c>
-      <c r="W22" s="29">
+      <c r="Q22" s="28">
+        <f t="shared" ref="Q22" si="9">Q5/M5-1</f>
+        <v>-2.770338945600781E-2</v>
+      </c>
+      <c r="W22" s="28">
         <f>W5/V5-1</f>
         <v>-0.137366539399013</v>
       </c>
-      <c r="X22" s="29">
+      <c r="X22" s="28">
         <f>X5/W5-1</f>
         <v>0.18793978595910144</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I23" s="43">
+      <c r="I23" s="42">
         <f>I5/H5-1</f>
         <v>0.17373497840556307</v>
       </c>
-      <c r="L23" s="43">
-        <f t="shared" ref="L23:M23" si="9">L5/K5-1</f>
+      <c r="L23" s="42">
+        <f t="shared" ref="L23:M23" si="10">L5/K5-1</f>
         <v>0.10678841317882548</v>
       </c>
-      <c r="M23" s="43">
-        <f t="shared" si="9"/>
+      <c r="M23" s="42">
+        <f t="shared" si="10"/>
         <v>4.6609238596288405E-2</v>
       </c>
-      <c r="N23" s="43">
-        <f t="shared" ref="N23:O23" si="10">N5/M5-1</f>
+      <c r="N23" s="42">
+        <f t="shared" ref="N23:O23" si="11">N5/M5-1</f>
         <v>0.28303614830527235</v>
       </c>
-      <c r="O23" s="43">
-        <f t="shared" si="10"/>
+      <c r="O23" s="42">
+        <f t="shared" si="11"/>
         <v>-0.3001593830644087</v>
       </c>
-      <c r="P23" s="43">
-        <f t="shared" ref="P23" si="11">P5/O5-1</f>
+      <c r="P23" s="42">
+        <f t="shared" ref="P23" si="12">P5/O5-1</f>
         <v>-9.4381873168282171E-3</v>
       </c>
-      <c r="V23" s="18" t="s">
+      <c r="Q23" s="42">
+        <f t="shared" ref="Q23" si="13">Q5/P5-1</f>
+        <v>9.3148476383414947E-2</v>
+      </c>
+      <c r="V23" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="W23" s="18" t="s">
+      <c r="W23" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="X23" s="18" t="s">
+      <c r="X23" s="17" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B24" s="33" t="s">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B24" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27">
+      <c r="I24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26">
         <f>L3/H3-1</f>
         <v>0.19856819367824641</v>
       </c>
-      <c r="M24" s="27">
+      <c r="M24" s="26">
         <f>M3/I3-1</f>
         <v>9.5761173990118964E-2</v>
       </c>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27">
+      <c r="N24" s="26"/>
+      <c r="O24" s="26">
         <f>O3/K3-1</f>
         <v>-3.068208531491301E-2</v>
       </c>
-      <c r="P24" s="27">
-        <f t="shared" ref="P24:P25" si="12">P3/L3-1</f>
+      <c r="P24" s="26">
+        <f t="shared" ref="P24:P25" si="14">P3/L3-1</f>
         <v>-0.15073189979066348</v>
       </c>
-      <c r="W24" s="27">
+      <c r="Q24" s="26">
+        <f t="shared" ref="Q24:Q25" si="15">Q3/M3-1</f>
+        <v>-0.12360260457849825</v>
+      </c>
+      <c r="W24" s="26">
         <f>W3/V3-1</f>
         <v>-0.15017970696506955</v>
       </c>
-      <c r="X24" s="27">
+      <c r="X24" s="26">
         <f>X3/W3-1</f>
         <v>0.17097618828260042</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B25" s="34" t="s">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B25" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="I25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27">
+      <c r="I25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26">
         <f>L4/H4-1</f>
         <v>0.30209231455329277</v>
       </c>
-      <c r="M25" s="27">
+      <c r="M25" s="26">
         <f>M4/I4-1</f>
         <v>0.11621689388550038</v>
       </c>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27">
+      <c r="N25" s="26"/>
+      <c r="O25" s="26">
         <f>O4/K4-1</f>
         <v>0.13254099593801705</v>
       </c>
-      <c r="P25" s="27">
-        <f t="shared" si="12"/>
+      <c r="P25" s="26">
+        <f t="shared" si="14"/>
         <v>5.0775329868395058E-2</v>
       </c>
-      <c r="W25" s="27">
+      <c r="Q25" s="26">
+        <f t="shared" si="15"/>
+        <v>0.10312943223046167</v>
+      </c>
+      <c r="W25" s="26">
         <f>W4/V4-1</f>
         <v>-0.11848208231966062</v>
       </c>
-      <c r="X25" s="27">
+      <c r="X25" s="26">
         <f>X4/W4-1</f>
         <v>0.21204227615827609</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="26">
         <f>H7/H5</f>
         <v>0.60660320078816821</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="26">
         <f>I7/I5</f>
         <v>0.63982275404683941</v>
       </c>
-      <c r="K27" s="27">
+      <c r="K27" s="26">
         <f>K7/K5</f>
         <v>0.63364580467235299</v>
       </c>
-      <c r="L27" s="27">
+      <c r="L27" s="26">
         <f>L7/L5</f>
         <v>0.65154072960629006</v>
       </c>
-      <c r="M27" s="27">
+      <c r="M27" s="26">
         <f>M7/M5</f>
         <v>0.63662114985195983</v>
       </c>
-      <c r="N27" s="27">
-        <f t="shared" ref="N27" si="13">N7/N5</f>
+      <c r="N27" s="26">
+        <f t="shared" ref="N27" si="16">N7/N5</f>
         <v>0.58305442014615716</v>
       </c>
-      <c r="O27" s="27">
+      <c r="O27" s="26">
         <f>O7/O5</f>
         <v>0.55310902822720542</v>
       </c>
-      <c r="P27" s="27">
-        <f t="shared" ref="P27" si="14">P7/P5</f>
+      <c r="P27" s="26">
+        <f t="shared" ref="P27:Q27" si="17">P7/P5</f>
         <v>0.57868116771892864</v>
       </c>
-      <c r="V27" s="27">
-        <f t="shared" ref="V27:W27" si="15">V7/V5</f>
+      <c r="Q27" s="26">
+        <f t="shared" si="17"/>
+        <v>0.59177987555733325</v>
+      </c>
+      <c r="V27" s="26">
+        <f t="shared" ref="V27:W27" si="18">V7/V5</f>
         <v>0.59367227764938779</v>
       </c>
-      <c r="W27" s="27">
-        <f t="shared" si="15"/>
+      <c r="W27" s="26">
+        <f t="shared" si="18"/>
         <v>0.60511124393034577</v>
       </c>
-      <c r="X27" s="27">
+      <c r="X27" s="26">
         <f>X7/X5</f>
         <v>0.6227146430910846</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="26">
         <f>H12/H5</f>
         <v>2.0252660640844914E-2</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="26">
         <f>I12/I5</f>
         <v>7.1512056336103663E-2</v>
       </c>
-      <c r="K28" s="27">
+      <c r="K28" s="26">
         <f>K12/K5</f>
         <v>7.3499657667918647E-2</v>
       </c>
-      <c r="L28" s="27">
+      <c r="L28" s="26">
         <f>L12/L5</f>
         <v>0.13272474995663991</v>
       </c>
-      <c r="M28" s="27">
+      <c r="M28" s="26">
         <f>M12/M5</f>
         <v>8.0351540059215978E-2</v>
       </c>
-      <c r="N28" s="27">
-        <f t="shared" ref="N28" si="16">N12/N5</f>
+      <c r="N28" s="26">
+        <f t="shared" ref="N28" si="19">N12/N5</f>
         <v>8.4498856075629139E-2</v>
       </c>
-      <c r="O28" s="27">
+      <c r="O28" s="26">
         <f>O12/O5</f>
         <v>-1.1966602769322474E-2</v>
       </c>
-      <c r="P28" s="27">
-        <f t="shared" ref="P28" si="17">P12/P5</f>
+      <c r="P28" s="26">
+        <f t="shared" ref="P28:Q28" si="20">P12/P5</f>
         <v>-2.721431490353244E-3</v>
       </c>
-      <c r="V28" s="27">
-        <f t="shared" ref="V28:W28" si="18">V12/V5</f>
+      <c r="Q28" s="26">
+        <f t="shared" si="20"/>
+        <v>1.9933324546293322E-2</v>
+      </c>
+      <c r="V28" s="26">
+        <f t="shared" ref="V28:W28" si="21">V12/V5</f>
         <v>1.9339383998059276E-2</v>
       </c>
-      <c r="W28" s="27">
-        <f t="shared" si="18"/>
+      <c r="W28" s="26">
+        <f t="shared" si="21"/>
         <v>-6.5492752250603924E-3</v>
       </c>
-      <c r="X28" s="27">
+      <c r="X28" s="26">
         <f>X12/X5</f>
         <v>9.2406527959732393E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="26">
         <f>H16/H5</f>
         <v>8.2940967568247981E-3</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="26">
         <f>I16/I5</f>
         <v>5.3715479252170475E-2</v>
       </c>
-      <c r="K29" s="27">
+      <c r="K29" s="26">
         <f>K16/K5</f>
         <v>5.4652836877163533E-2</v>
       </c>
-      <c r="L29" s="27">
+      <c r="L29" s="26">
         <f>L16/L5</f>
         <v>0.12771694513499451</v>
       </c>
-      <c r="M29" s="27">
+      <c r="M29" s="26">
         <f>M16/M5</f>
         <v>5.4220248353882131E-2</v>
       </c>
-      <c r="N29" s="27">
-        <f t="shared" ref="N29" si="19">N16/N5</f>
+      <c r="N29" s="26">
+        <f t="shared" ref="N29" si="22">N16/N5</f>
         <v>5.8402570105730238E-2</v>
       </c>
-      <c r="O29" s="27">
+      <c r="O29" s="26">
         <f>O16/O5</f>
         <v>-1.8266109882105801E-2</v>
       </c>
-      <c r="P29" s="27">
-        <f t="shared" ref="P29" si="20">P16/P5</f>
+      <c r="P29" s="26">
+        <f t="shared" ref="P29:Q29" si="23">P16/P5</f>
         <v>-1.8310973542121304E-2</v>
       </c>
-      <c r="V29" s="27">
-        <f t="shared" ref="V29:W29" si="21">V16/V5</f>
+      <c r="Q29" s="26">
+        <f t="shared" si="23"/>
+        <v>-8.1583121611117728E-4</v>
+      </c>
+      <c r="V29" s="26">
+        <f t="shared" ref="V29:W29" si="24">V16/V5</f>
         <v>1.2409355262784E-2</v>
       </c>
-      <c r="W29" s="27">
-        <f t="shared" si="21"/>
+      <c r="W29" s="26">
+        <f t="shared" si="24"/>
         <v>-3.4860996280777067E-2</v>
       </c>
-      <c r="X29" s="27">
+      <c r="X29" s="26">
         <f>X16/X5</f>
         <v>7.2739799524236287E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="26">
         <f>H18/H5</f>
         <v>7.8244034321979742E-3</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="26">
         <f>I18/I5</f>
         <v>5.1570666575571134E-2</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K30" s="26">
         <f>K18/K5</f>
         <v>5.3452435036888638E-2</v>
       </c>
-      <c r="L30" s="27">
+      <c r="L30" s="26">
         <f>L18/L5</f>
         <v>0.12545528126264671</v>
       </c>
-      <c r="M30" s="27">
+      <c r="M30" s="26">
         <f>M18/M5</f>
         <v>5.218193468558039E-2</v>
       </c>
-      <c r="N30" s="27">
-        <f t="shared" ref="N30" si="22">N18/N5</f>
+      <c r="N30" s="26">
+        <f t="shared" ref="N30" si="25">N18/N5</f>
         <v>5.6407483340552046E-2</v>
       </c>
-      <c r="O30" s="27">
+      <c r="O30" s="26">
         <f>O18/O5</f>
         <v>-2.0263004421958795E-2</v>
       </c>
-      <c r="P30" s="27">
-        <f t="shared" ref="P30" si="23">P18/P5</f>
+      <c r="P30" s="26">
+        <f t="shared" ref="P30:Q30" si="26">P18/P5</f>
         <v>-2.0909437566684987E-2</v>
       </c>
-      <c r="V30" s="27">
-        <f t="shared" ref="V30:W30" si="24">V18/V5</f>
+      <c r="Q30" s="26">
+        <f t="shared" si="26"/>
+        <v>-2.5156689588720959E-3</v>
+      </c>
+      <c r="V30" s="26">
+        <f t="shared" ref="V30:W30" si="27">V18/V5</f>
         <v>1.0863154013181798E-2</v>
       </c>
-      <c r="W30" s="27">
-        <f t="shared" si="24"/>
+      <c r="W30" s="26">
+        <f t="shared" si="27"/>
         <v>-3.6482237062709783E-2</v>
       </c>
-      <c r="X30" s="27">
+      <c r="X30" s="26">
         <f>X18/X5</f>
         <v>7.0839330655726326E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="26">
         <f>H15/H14</f>
         <v>0.17785663591199563</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I31" s="26">
         <f>I15/I14</f>
         <v>0.11602786756881554</v>
       </c>
-      <c r="K31" s="27">
+      <c r="K31" s="26">
         <f>K15/K14</f>
         <v>0.12536096831671009</v>
       </c>
-      <c r="L31" s="27">
+      <c r="L31" s="26">
         <f>L15/L14</f>
         <v>-6.7084009583429929E-2</v>
       </c>
-      <c r="M31" s="27">
+      <c r="M31" s="26">
         <f>M15/M14</f>
         <v>0.25027115381677661</v>
       </c>
-      <c r="N31" s="27">
-        <f t="shared" ref="N31" si="25">N15/N14</f>
+      <c r="N31" s="26">
+        <f t="shared" ref="N31" si="28">N15/N14</f>
         <v>0.25608177769978241</v>
       </c>
-      <c r="O31" s="27">
+      <c r="O31" s="26">
         <f>O15/O14</f>
         <v>0.12839781600422653</v>
       </c>
-      <c r="P31" s="27">
-        <f t="shared" ref="P31" si="26">P15/P14</f>
+      <c r="P31" s="26">
+        <f t="shared" ref="P31:Q31" si="29">P15/P14</f>
         <v>-0.61857707509881543</v>
       </c>
-      <c r="V31" s="27">
-        <f t="shared" ref="V31:W31" si="27">V15/V14</f>
+      <c r="Q31" s="26">
+        <f t="shared" si="29"/>
+        <v>1.070062451209991</v>
+      </c>
+      <c r="V31" s="26">
+        <f t="shared" ref="V31:W31" si="30">V15/V14</f>
         <v>0.27868957661516464</v>
       </c>
-      <c r="W31" s="27">
-        <f t="shared" si="27"/>
+      <c r="W31" s="26">
+        <f t="shared" si="30"/>
         <v>-1.2352748086904748</v>
       </c>
-      <c r="X31" s="27">
+      <c r="X31" s="26">
         <f>X15/X14</f>
         <v>0.12592645335853514</v>
       </c>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B33" s="28" t="s">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B33" s="27" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B34" s="34" t="s">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B34" s="33" t="s">
         <v>122</v>
       </c>
       <c r="K34" s="1">
@@ -3188,13 +3351,17 @@
         <f>358+155</f>
         <v>513</v>
       </c>
+      <c r="Q34" s="1">
+        <f>367+156</f>
+        <v>523</v>
+      </c>
       <c r="X34" s="1">
         <f>154+351</f>
         <v>505</v>
       </c>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B35" s="34" t="s">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B35" s="33" t="s">
         <v>123</v>
       </c>
       <c r="K35" s="1">
@@ -3209,12 +3376,16 @@
         <f>172+49</f>
         <v>221</v>
       </c>
+      <c r="Q35" s="1">
+        <f>174+54</f>
+        <v>228</v>
+      </c>
       <c r="X35" s="1">
         <f>51+173</f>
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>124</v>
       </c>
@@ -3230,527 +3401,940 @@
         <f>P34+P35</f>
         <v>734</v>
       </c>
+      <c r="Q36" s="1">
+        <f>Q34+Q35</f>
+        <v>751</v>
+      </c>
       <c r="X36" s="1">
         <f>X34+X35</f>
         <v>729</v>
       </c>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B38" s="28" t="s">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B38" s="27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O39" s="25">
+      <c r="O39" s="24">
         <v>468.37799999999999</v>
       </c>
-      <c r="P39" s="25">
+      <c r="P39" s="24">
         <v>369.95600000000002</v>
       </c>
-      <c r="W39" s="25">
+      <c r="Q39" s="24">
+        <v>257.33199999999999</v>
+      </c>
+      <c r="W39" s="24">
         <v>1104.8620000000001</v>
       </c>
-      <c r="X39" s="25">
+      <c r="X39" s="24">
         <v>823.13900000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O40" s="26">
+      <c r="O40" s="25">
         <v>88.807000000000002</v>
       </c>
-      <c r="P40" s="26">
+      <c r="P40" s="25">
         <v>79.72</v>
       </c>
-      <c r="W40" s="26">
+      <c r="Q40" s="25">
+        <v>108.468</v>
+      </c>
+      <c r="W40" s="25">
         <v>83.856999999999999</v>
       </c>
-      <c r="X40" s="26">
+      <c r="X40" s="25">
         <v>69.102000000000004</v>
       </c>
     </row>
-    <row r="41" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O41" s="25">
+      <c r="O41" s="24">
         <v>562.51</v>
       </c>
-      <c r="P41" s="25">
+      <c r="P41" s="24">
         <v>708.024</v>
       </c>
-      <c r="W41" s="25">
+      <c r="Q41" s="24">
+        <v>741.96299999999997</v>
+      </c>
+      <c r="W41" s="24">
         <v>404.053</v>
       </c>
-      <c r="X41" s="25">
+      <c r="X41" s="24">
         <v>525.86400000000003</v>
       </c>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O42" s="26">
+      <c r="O42" s="25">
         <v>93.179000000000002</v>
       </c>
-      <c r="P42" s="26">
+      <c r="P42" s="25">
         <v>104.887</v>
       </c>
-      <c r="W42" s="26">
+      <c r="Q42" s="25">
+        <v>112.602</v>
+      </c>
+      <c r="W42" s="25">
         <v>68.856999999999999</v>
       </c>
-      <c r="X42" s="26">
+      <c r="X42" s="25">
         <v>89.653999999999996</v>
       </c>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K43" s="26">
+      <c r="K43" s="25">
         <f>SUM(K39:K42)</f>
         <v>0</v>
       </c>
-      <c r="L43" s="26">
-        <f t="shared" ref="L43:N43" si="28">SUM(L39:L42)</f>
+      <c r="L43" s="25">
+        <f t="shared" ref="L43:N43" si="31">SUM(L39:L42)</f>
         <v>0</v>
       </c>
-      <c r="M43" s="26">
-        <f t="shared" si="28"/>
+      <c r="M43" s="25">
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="N43" s="26">
-        <f t="shared" si="28"/>
+      <c r="N43" s="25">
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="O43" s="26">
+      <c r="O43" s="25">
         <f>SUM(O39:O42)</f>
         <v>1212.874</v>
       </c>
-      <c r="P43" s="26">
+      <c r="P43" s="25">
         <f>SUM(P39:P42)</f>
         <v>1262.587</v>
       </c>
-      <c r="W43" s="26">
+      <c r="Q43" s="25">
+        <f>SUM(Q39:Q42)</f>
+        <v>1220.365</v>
+      </c>
+      <c r="W43" s="25">
         <f>SUM(W39:W42)</f>
         <v>1661.6289999999999</v>
       </c>
-      <c r="X43" s="26">
+      <c r="X43" s="25">
         <f>SUM(X39:X42)</f>
         <v>1507.759</v>
       </c>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O44" s="26">
+      <c r="O44" s="25">
         <v>497.976</v>
       </c>
-      <c r="P44" s="26">
+      <c r="P44" s="25">
         <v>511.18099999999998</v>
       </c>
-      <c r="W44" s="26">
+      <c r="Q44" s="25">
+        <v>542.13800000000003</v>
+      </c>
+      <c r="W44" s="25">
         <v>550.58699999999999</v>
       </c>
-      <c r="X44" s="26">
+      <c r="X44" s="25">
         <v>508.33600000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O45" s="26">
+      <c r="O45" s="25">
         <v>671.99099999999999</v>
       </c>
-      <c r="P45" s="26">
+      <c r="P45" s="25">
         <v>740.62699999999995</v>
       </c>
-      <c r="W45" s="26">
+      <c r="Q45" s="25">
+        <v>713.16600000000005</v>
+      </c>
+      <c r="W45" s="25">
         <v>893.98900000000003</v>
       </c>
-      <c r="X45" s="26">
+      <c r="X45" s="25">
         <v>698.23099999999999</v>
       </c>
     </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O46" s="26">
+      <c r="O46" s="25">
         <v>224.46199999999999</v>
       </c>
-      <c r="P46" s="26">
+      <c r="P46" s="25">
         <v>219.59800000000001</v>
       </c>
-      <c r="W46" s="26">
+      <c r="Q46" s="25">
+        <v>218.32499999999999</v>
+      </c>
+      <c r="W46" s="25">
         <v>208.697</v>
       </c>
-      <c r="X46" s="26">
+      <c r="X46" s="25">
         <v>225.16499999999999</v>
       </c>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K47" s="26">
+      <c r="K47" s="25">
         <f>K43+K44+K45+K46</f>
         <v>0</v>
       </c>
-      <c r="L47" s="26">
-        <f t="shared" ref="L47:N47" si="29">L43+L44+L45+L46</f>
+      <c r="L47" s="25">
+        <f t="shared" ref="L47:N47" si="32">L43+L44+L45+L46</f>
         <v>0</v>
       </c>
-      <c r="M47" s="26">
-        <f t="shared" si="29"/>
+      <c r="M47" s="25">
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="N47" s="26">
-        <f t="shared" si="29"/>
+      <c r="N47" s="25">
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="O47" s="26">
+      <c r="O47" s="25">
         <f>O43+O44+O45+O46</f>
         <v>2607.3029999999999</v>
       </c>
-      <c r="P47" s="26">
+      <c r="P47" s="25">
         <f>P43+P44+P45+P46</f>
         <v>2733.9929999999999</v>
       </c>
-      <c r="W47" s="26">
+      <c r="Q47" s="25">
+        <f>Q43+Q44+Q45+Q46</f>
+        <v>2693.9940000000001</v>
+      </c>
+      <c r="W47" s="25">
         <f>W43+W44+W45+W46</f>
         <v>3314.902</v>
       </c>
-      <c r="X47" s="26">
+      <c r="X47" s="25">
         <f>X43+X44+X45+X46</f>
         <v>2939.491</v>
       </c>
     </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="O48" s="26"/>
-      <c r="W48" s="26"/>
-      <c r="X48" s="26"/>
-    </row>
-    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="O48" s="25"/>
+      <c r="Q48" s="25"/>
+      <c r="W48" s="25"/>
+      <c r="X48" s="25"/>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O49" s="26">
+      <c r="O49" s="25">
         <v>311.35199999999998</v>
       </c>
-      <c r="P49" s="26">
+      <c r="P49" s="25">
         <v>408.29700000000003</v>
       </c>
-      <c r="W49" s="26">
+      <c r="Q49" s="25">
+        <v>322.12799999999999</v>
+      </c>
+      <c r="W49" s="25">
         <v>289.39600000000002</v>
       </c>
-      <c r="X49" s="26">
+      <c r="X49" s="25">
         <v>374.82900000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O50" s="26">
+      <c r="O50" s="25">
         <v>320.68099999999998</v>
       </c>
-      <c r="P50" s="26">
+      <c r="P50" s="25">
         <v>342.69</v>
       </c>
-      <c r="W50" s="26">
+      <c r="Q50" s="25">
+        <v>378.36599999999999</v>
+      </c>
+      <c r="W50" s="25">
         <v>396.36500000000001</v>
       </c>
-      <c r="X50" s="26">
+      <c r="X50" s="25">
         <v>395.815</v>
       </c>
     </row>
-    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O51" s="26">
+      <c r="O51" s="25">
         <v>195.59899999999999</v>
       </c>
-      <c r="P51" s="26">
+      <c r="P51" s="25">
         <v>202.66900000000001</v>
       </c>
-      <c r="W51" s="26">
+      <c r="Q51" s="25">
+        <v>211.304</v>
+      </c>
+      <c r="W51" s="25">
         <v>248.846</v>
       </c>
-      <c r="X51" s="26">
+      <c r="X51" s="25">
         <v>222.82300000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O52" s="26">
+      <c r="O52" s="25">
         <v>25.4</v>
       </c>
-      <c r="P52" s="26">
+      <c r="P52" s="25">
         <v>5.5819999999999999</v>
       </c>
-      <c r="W52" s="26">
+      <c r="Q52" s="25">
+        <v>23.693999999999999</v>
+      </c>
+      <c r="W52" s="25">
         <v>24.792000000000002</v>
       </c>
-      <c r="X52" s="26">
+      <c r="X52" s="25">
         <v>21.773</v>
       </c>
     </row>
-    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K53" s="26">
+      <c r="K53" s="25">
         <f>SUM(K49:K52)</f>
         <v>0</v>
       </c>
-      <c r="L53" s="26">
-        <f t="shared" ref="L53:N53" si="30">SUM(L49:L52)</f>
+      <c r="L53" s="25">
+        <f t="shared" ref="L53:N53" si="33">SUM(L49:L52)</f>
         <v>0</v>
       </c>
-      <c r="M53" s="26">
-        <f t="shared" si="30"/>
+      <c r="M53" s="25">
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="N53" s="26">
-        <f t="shared" si="30"/>
+      <c r="N53" s="25">
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="O53" s="26">
+      <c r="O53" s="25">
         <f>SUM(O49:O52)</f>
         <v>853.03199999999981</v>
       </c>
-      <c r="P53" s="26">
+      <c r="P53" s="25">
         <f>SUM(P49:P52)</f>
         <v>959.23800000000006</v>
       </c>
-      <c r="W53" s="26">
+      <c r="Q53" s="25">
+        <f>SUM(Q49:Q52)</f>
+        <v>935.49199999999985</v>
+      </c>
+      <c r="W53" s="25">
         <f>SUM(W49:W52)</f>
         <v>959.399</v>
       </c>
-      <c r="X53" s="26">
+      <c r="X53" s="25">
         <f>SUM(X49:X52)</f>
         <v>1015.24</v>
       </c>
     </row>
-    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O54" s="26">
+      <c r="O54" s="25">
         <v>662.322</v>
       </c>
-      <c r="P54" s="26">
+      <c r="P54" s="25">
         <v>714.26499999999999</v>
       </c>
-      <c r="W54" s="26">
+      <c r="Q54" s="25">
+        <v>708.51199999999994</v>
+      </c>
+      <c r="W54" s="25">
         <v>957.55799999999999</v>
       </c>
-      <c r="X54" s="26">
+      <c r="X54" s="25">
         <v>697.26400000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B55" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O55" s="25">
+      <c r="O55" s="24">
         <v>303.90100000000001</v>
       </c>
-      <c r="P55" s="25">
+      <c r="P55" s="24">
         <v>304.21899999999999</v>
       </c>
-      <c r="W55" s="25">
+      <c r="Q55" s="24">
+        <v>296.53199999999998</v>
+      </c>
+      <c r="W55" s="24">
         <v>343.91</v>
       </c>
-      <c r="X55" s="25">
+      <c r="X55" s="24">
         <v>303.57400000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O56" s="26">
+      <c r="O56" s="25">
         <v>83.242999999999995</v>
       </c>
-      <c r="P56" s="26">
+      <c r="P56" s="25">
         <v>83.415000000000006</v>
       </c>
-      <c r="W56" s="26">
+      <c r="Q56" s="25">
+        <v>97.393000000000001</v>
+      </c>
+      <c r="W56" s="25">
         <v>104.693</v>
       </c>
-      <c r="X56" s="26">
+      <c r="X56" s="25">
         <v>86.088999999999999</v>
       </c>
     </row>
-    <row r="57" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K57" s="26">
+      <c r="K57" s="25">
         <f>K53+K54+K55+K56</f>
         <v>0</v>
       </c>
-      <c r="L57" s="26">
-        <f t="shared" ref="L57:N57" si="31">L53+L54+L55+L56</f>
+      <c r="L57" s="25">
+        <f t="shared" ref="L57:N57" si="34">L53+L54+L55+L56</f>
         <v>0</v>
       </c>
-      <c r="M57" s="26">
-        <f t="shared" si="31"/>
+      <c r="M57" s="25">
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="N57" s="26">
-        <f t="shared" si="31"/>
+      <c r="N57" s="25">
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
-      <c r="O57" s="26">
+      <c r="O57" s="25">
         <f>O53+O54+O55+O56</f>
         <v>1902.4979999999998</v>
       </c>
-      <c r="P57" s="26">
+      <c r="P57" s="25">
         <f>P53+P54+P55+P56</f>
         <v>2061.1370000000002</v>
       </c>
-      <c r="W57" s="26">
+      <c r="Q57" s="25">
+        <f>Q53+Q54+Q55+Q56</f>
+        <v>2037.9289999999999</v>
+      </c>
+      <c r="W57" s="25">
         <f>W53+W54+W55+W56</f>
         <v>2365.56</v>
       </c>
-      <c r="X57" s="26">
+      <c r="X57" s="25">
         <f>X53+X54+X55+X56</f>
         <v>2102.1669999999999</v>
       </c>
     </row>
-    <row r="58" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="W58" s="26"/>
-      <c r="X58" s="26"/>
-    </row>
-    <row r="59" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Q58" s="25"/>
+      <c r="W58" s="25"/>
+      <c r="X58" s="25"/>
+    </row>
+    <row r="59" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O59" s="26">
+      <c r="O59" s="25">
         <v>704.80499999999995</v>
       </c>
-      <c r="P59" s="26">
+      <c r="P59" s="25">
         <v>672.92700000000002</v>
       </c>
-      <c r="W59" s="26">
+      <c r="Q59" s="25">
+        <v>656.06500000000005</v>
+      </c>
+      <c r="W59" s="25">
         <v>949.31200000000001</v>
       </c>
-      <c r="X59" s="26">
+      <c r="X59" s="25">
         <v>837.32399999999996</v>
       </c>
     </row>
-    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O60" s="26">
+      <c r="O60" s="25">
         <f>O59+O57</f>
         <v>2607.3029999999999</v>
       </c>
-      <c r="P60" s="26">
+      <c r="P60" s="25">
         <f>P59+P57</f>
         <v>2734.0640000000003</v>
       </c>
-      <c r="W60" s="26">
+      <c r="Q60" s="25">
+        <f>Q59+Q57</f>
+        <v>2693.9939999999997</v>
+      </c>
+      <c r="W60" s="25">
         <f>W59+W57</f>
         <v>3314.8719999999998</v>
       </c>
-      <c r="X60" s="26">
+      <c r="X60" s="25">
         <f>X59+X57</f>
         <v>2939.491</v>
       </c>
     </row>
-    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="X61" s="26"/>
-    </row>
-    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="X61" s="25"/>
+    </row>
+    <row r="62" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="X62" s="26"/>
-    </row>
-    <row r="63" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="X62" s="25"/>
+    </row>
+    <row r="63" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="O63" s="26">
+      <c r="O63" s="25">
         <f>O47-O57</f>
         <v>704.80500000000006</v>
       </c>
-      <c r="P63" s="26">
-        <f t="shared" ref="P63" si="32">P47-P57</f>
+      <c r="P63" s="25">
+        <f t="shared" ref="P63:Q63" si="35">P47-P57</f>
         <v>672.85599999999977</v>
       </c>
-      <c r="W63" s="26">
+      <c r="Q63" s="25">
+        <f t="shared" si="35"/>
+        <v>656.06500000000028</v>
+      </c>
+      <c r="W63" s="25">
         <f>W47-W57</f>
         <v>949.3420000000001</v>
       </c>
-      <c r="X63" s="26">
+      <c r="X63" s="25">
         <f>X47-X57</f>
         <v>837.32400000000007</v>
       </c>
     </row>
-    <row r="64" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="O64" s="30">
+    <row r="64" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="O64" s="29">
         <f>O63/O20</f>
         <v>13.533901722449452</v>
       </c>
-      <c r="P64" s="30">
-        <f t="shared" ref="P64" si="33">P63/P20</f>
+      <c r="P64" s="29">
+        <f t="shared" ref="P64:Q64" si="36">P63/P20</f>
         <v>13.339465910667904</v>
       </c>
-      <c r="W64" s="26">
+      <c r="Q64" s="29">
+        <f t="shared" si="36"/>
+        <v>13.257588004688202</v>
+      </c>
+      <c r="W64" s="25">
         <f>W63/W20</f>
         <v>15.177087496602773</v>
       </c>
-      <c r="X64" s="26">
+      <c r="X64" s="25">
         <f>X63/X20</f>
         <v>14.049767605751969</v>
       </c>
     </row>
-    <row r="66" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B66" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="X66" s="29">
+      <c r="X66" s="28">
         <f>X41/W41-1</f>
         <v>0.30147282658463137</v>
       </c>
     </row>
-    <row r="67" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B67" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="P67" s="27">
+      <c r="P67" s="26">
         <f>P41/O41-1</f>
         <v>0.25868695667632569</v>
       </c>
-    </row>
-    <row r="69" spans="2:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="3" t="s">
+      <c r="Q67" s="26">
+        <f>Q41/P41-1</f>
+        <v>4.7934815768956973E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A68" s="61">
+        <f>AVERAGE( C68:AK68)</f>
+        <v>0.25420875419415584</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="O68" s="26">
+        <f>O43/SUM(L5:O5)</f>
+        <v>0.32394057356525224</v>
+      </c>
+      <c r="P68" s="26">
+        <f>P43/SUM(M5:P5)</f>
+        <v>0.34268772429232053</v>
+      </c>
+      <c r="Q68" s="26">
+        <f>Q43/SUM(N5:Q5)</f>
+        <v>0.33349775502898105</v>
+      </c>
+      <c r="W68" s="26">
+        <f t="shared" ref="W68:X68" si="37">W41/W5</f>
+        <v>0.12928107394163404</v>
+      </c>
+      <c r="X68" s="26">
+        <f>X41/X5</f>
+        <v>0.14163664414259119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B70" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="O70" s="31">
+        <f t="shared" ref="O70:Q70" si="38">O39</f>
+        <v>468.37799999999999</v>
+      </c>
+      <c r="P70" s="31">
+        <f t="shared" si="38"/>
+        <v>369.95600000000002</v>
+      </c>
+      <c r="Q70" s="31">
+        <f>Q39</f>
+        <v>257.33199999999999</v>
+      </c>
+      <c r="W70" s="31">
+        <f>W39</f>
+        <v>1104.8620000000001</v>
+      </c>
+      <c r="X70" s="31">
+        <f>X39</f>
+        <v>823.13900000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B71" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="O71" s="31">
+        <f t="shared" ref="O71:Q71" si="39">O55</f>
+        <v>303.90100000000001</v>
+      </c>
+      <c r="P71" s="31">
+        <f t="shared" si="39"/>
+        <v>304.21899999999999</v>
+      </c>
+      <c r="Q71" s="31">
+        <f>Q55</f>
+        <v>296.53199999999998</v>
+      </c>
+      <c r="W71" s="31">
+        <f>W55</f>
+        <v>343.91</v>
+      </c>
+      <c r="X71" s="31">
+        <f>X55</f>
+        <v>303.57400000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="B72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O72" s="25">
+        <f t="shared" ref="O72:P72" si="40">O70-O71</f>
+        <v>164.47699999999998</v>
+      </c>
+      <c r="P72" s="25">
+        <f t="shared" si="40"/>
+        <v>65.737000000000023</v>
+      </c>
+      <c r="Q72" s="25">
+        <f>Q70-Q71</f>
+        <v>-39.199999999999989</v>
+      </c>
+      <c r="W72" s="25">
+        <f>W70-W71</f>
+        <v>760.952</v>
+      </c>
+      <c r="X72" s="25">
+        <f>X70-X71</f>
+        <v>519.56500000000005</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B74" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="X69" s="29">
+      <c r="X74" s="28">
         <f>X39/W39-1</f>
         <v>-0.25498478543021663</v>
       </c>
     </row>
-    <row r="70" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B70" s="1" t="s">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="B75" s="1" t="s">
         <v>135</v>
+      </c>
+      <c r="P75" s="26">
+        <f t="shared" ref="P75:Q75" si="41">P70/O70-1</f>
+        <v>-0.21013369543402971</v>
+      </c>
+      <c r="Q75" s="26">
+        <f>Q70/P70-1</f>
+        <v>-0.30442539112759359</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="B77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O77" s="1">
+        <v>34.58</v>
+      </c>
+      <c r="P77" s="1">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="V77" s="1">
+        <v>17.23</v>
+      </c>
+      <c r="W77" s="1">
+        <v>20.49</v>
+      </c>
+      <c r="X77" s="1">
+        <v>34.979999999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="B78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O78" s="25">
+        <f t="shared" ref="O78:P78" si="42">O77*O20</f>
+        <v>1800.8226599999998</v>
+      </c>
+      <c r="P78" s="25">
+        <f t="shared" si="42"/>
+        <v>853.46172000000013</v>
+      </c>
+      <c r="Q78" s="25">
+        <f>Q77*Q20</f>
+        <v>869.9638799999999</v>
+      </c>
+      <c r="V78" s="25"/>
+      <c r="W78" s="25">
+        <f t="shared" ref="W78" si="43">W77*W20</f>
+        <v>1281.6699899999999</v>
+      </c>
+      <c r="X78" s="25">
+        <f>X77*X20</f>
+        <v>2084.7030599999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="B79" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O79" s="25">
+        <f t="shared" ref="O79:P79" si="44">O78-O72</f>
+        <v>1636.34566</v>
+      </c>
+      <c r="P79" s="25">
+        <f t="shared" si="44"/>
+        <v>787.72472000000016</v>
+      </c>
+      <c r="Q79" s="25">
+        <f>Q78-Q72</f>
+        <v>909.16387999999984</v>
+      </c>
+      <c r="V79" s="25"/>
+      <c r="W79" s="25">
+        <f t="shared" ref="W79" si="45">W78-W72</f>
+        <v>520.71798999999987</v>
+      </c>
+      <c r="X79" s="25">
+        <f>X78-X72</f>
+        <v>1565.1380599999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A81" s="60">
+        <f>AVERAGE( C81:AK81)</f>
+        <v>1.797859412227653</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O81" s="59">
+        <f t="shared" ref="O81:Q81" si="46">O77/O64</f>
+        <v>2.5550651031136269</v>
+      </c>
+      <c r="P81" s="59">
+        <f t="shared" si="46"/>
+        <v>1.2684166002829735</v>
+      </c>
+      <c r="Q81" s="59">
+        <f>Q77/Q64</f>
+        <v>1.3260330607485531</v>
+      </c>
+      <c r="V81" s="59"/>
+      <c r="W81" s="59">
+        <f t="shared" ref="V81:X81" si="47">W77/W64</f>
+        <v>1.3500614004226084</v>
+      </c>
+      <c r="X81" s="59">
+        <f>X77/X64</f>
+        <v>2.4897208965705029</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A82" s="60">
+        <f>AVERAGE( C82:AK82)</f>
+        <v>0.3843875677046612</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O82" s="59">
+        <f t="shared" ref="O82:P82" si="48">O78/SUM(L5:O5)</f>
+        <v>0.48097290021032946</v>
+      </c>
+      <c r="P82" s="59">
+        <f t="shared" si="48"/>
+        <v>0.23164412004670545</v>
+      </c>
+      <c r="Q82" s="59">
+        <f>Q78/SUM(N5:Q5)</f>
+        <v>0.23774116836872725</v>
+      </c>
+      <c r="W82" s="59">
+        <f>W78/W5</f>
+        <v>0.41008400567738235</v>
+      </c>
+      <c r="X82" s="59">
+        <f>X78/X5</f>
+        <v>0.56149564422016129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A83" s="60">
+        <f>AVERAGE( C83:AK83)</f>
+        <v>0.29749280159584623</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O83" s="59">
+        <f t="shared" ref="O83:P83" si="49">O79/SUM(L5:O5)</f>
+        <v>0.43704354421927688</v>
+      </c>
+      <c r="P83" s="59">
+        <f t="shared" si="49"/>
+        <v>0.21380197298531148</v>
+      </c>
+      <c r="Q83" s="59">
+        <f>Q79/SUM(N5:Q5)</f>
+        <v>0.24845362898267145</v>
+      </c>
+      <c r="W83" s="59">
+        <f t="shared" ref="W83:X83" si="50">W79/W5</f>
+        <v>0.16660928385120033</v>
+      </c>
+      <c r="X83" s="59">
+        <f>X79/X5</f>
+        <v>0.42155557794077081</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A84" s="60">
+        <f>AVERAGE( C84:AK84)</f>
+        <v>15.362787955012152</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O84" s="59">
+        <f t="shared" ref="O84:P84" si="51">O77/SUM(L19:O19)</f>
+        <v>10.314417228677181</v>
+      </c>
+      <c r="P84" s="59">
+        <f t="shared" si="51"/>
+        <v>13.508368512238665</v>
+      </c>
+      <c r="Q84" s="59">
+        <f>Q77/SUM(N19:Q19)</f>
+        <v>43.463212244578067</v>
+      </c>
+      <c r="V84" s="59">
+        <f t="shared" ref="V84:X84" si="52">V77/V19</f>
+        <v>28.205052085979538</v>
+      </c>
+      <c r="W84" s="59">
+        <f t="shared" si="52"/>
+        <v>-11.240648564738059</v>
+      </c>
+      <c r="X84" s="59">
+        <f>X77/X19</f>
+        <v>7.9263262233375249</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="B85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O85" s="59">
+        <f t="shared" ref="O85:P85" si="53">O79/SUM(L16:O16)</f>
+        <v>7.6999428743518044</v>
+      </c>
+      <c r="P85" s="59">
+        <f t="shared" si="53"/>
+        <v>9.0215392367950873</v>
+      </c>
+      <c r="Q85" s="59">
+        <f>Q79/SUM(N16:Q16)</f>
+        <v>24.23144669509588</v>
+      </c>
+      <c r="W85" s="59"/>
+      <c r="X85" s="59">
+        <f>X79/X16</f>
+        <v>5.7953909785015574</v>
       </c>
     </row>
   </sheetData>
@@ -3760,11 +4344,12 @@
     <hyperlink ref="M1" r:id="rId3" location="id3a4d98ceaf340b49a9b4120a6f6242d_31" xr:uid="{F8710F00-6532-1246-AC65-F36142AF7599}"/>
     <hyperlink ref="L1" r:id="rId4" location="ib223de12289d413dbeacbd98f83fd0f5_16" xr:uid="{CB4C7934-1202-5C47-ADA3-87001AAE1270}"/>
     <hyperlink ref="P1" r:id="rId5" xr:uid="{1A8AB90C-3113-8A4A-A39C-004613218F30}"/>
+    <hyperlink ref="Q1" r:id="rId6" xr:uid="{6B7AEDDE-9C9E-C147-91CE-AB521C7B1DD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="N7 N15:N17 N14 N12" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reconcile D&A writeoffs back into NI
</commit_message>
<xml_diff>
--- a/$ANF.xlsx
+++ b/$ANF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108F50CD-6E1B-C249-9C43-CC6AD0EC0677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7B1450-C647-3A43-B69A-CE404422B961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18900" activeTab="1" xr2:uid="{BED0471A-CBC0-4084-A037-CD3E53E820DA}"/>
   </bookViews>
@@ -503,7 +503,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="#.#\x"/>
     <numFmt numFmtId="167" formatCode="0.#\x"/>
-    <numFmt numFmtId="170" formatCode="0.0\x"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -590,7 +590,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +612,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,7 +716,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -799,6 +805,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,18 +820,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -832,20 +834,37 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1356,28 +1375,28 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-      <c r="H5" s="46" t="s">
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
+      <c r="H5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="48"/>
-      <c r="S5" s="46" t="s">
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="54"/>
+      <c r="S5" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="T5" s="47"/>
-      <c r="U5" s="47"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="48"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="54"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
@@ -1439,7 +1458,7 @@
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="62">
+      <c r="C8" s="49">
         <f>C6*C7</f>
         <v>1119.3733199999999</v>
       </c>
@@ -1462,7 +1481,7 @@
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="62">
+      <c r="C9" s="49">
         <f>'Financial Model'!Q39</f>
         <v>257.33199999999999</v>
       </c>
@@ -1490,7 +1509,7 @@
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="62">
+      <c r="C10" s="49">
         <f>'Financial Model'!Q40</f>
         <v>108.468</v>
       </c>
@@ -1518,7 +1537,7 @@
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="62">
+      <c r="C11" s="49">
         <f>C9-C10</f>
         <v>148.86399999999998</v>
       </c>
@@ -1544,7 +1563,7 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="63">
+      <c r="C12" s="50">
         <f>C8-C11</f>
         <v>970.50931999999989</v>
       </c>
@@ -1606,11 +1625,11 @@
       <c r="W14" s="9"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
       <c r="H15" s="6"/>
       <c r="I15" s="41" t="s">
         <v>127</v>
@@ -1633,10 +1652,10 @@
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="52"/>
+      <c r="D16" s="60"/>
       <c r="H16" s="6"/>
       <c r="I16" s="41" t="s">
         <v>128</v>
@@ -1659,10 +1678,10 @@
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="52"/>
+      <c r="D17" s="60"/>
       <c r="H17" s="6"/>
       <c r="I17" s="41" t="s">
         <v>129</v>
@@ -1685,10 +1704,10 @@
       <c r="B18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="52"/>
+      <c r="D18" s="60"/>
       <c r="H18" s="6"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1707,8 +1726,8 @@
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B19" s="13"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="56"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
       <c r="H19" s="6"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1757,11 +1776,11 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="54"/>
       <c r="H22" s="6"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1775,10 +1794,10 @@
       <c r="B23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="52"/>
+      <c r="D23" s="60"/>
       <c r="H23" s="7"/>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
@@ -1792,25 +1811,25 @@
       <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C24" s="59">
         <v>1892</v>
       </c>
-      <c r="D24" s="52"/>
+      <c r="D24" s="60"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B25" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="51">
+      <c r="C25" s="59">
         <f>'Financial Model'!Q36</f>
         <v>751</v>
       </c>
-      <c r="D25" s="52"/>
+      <c r="D25" s="60"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B26" s="6"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B27" s="6" t="s">
@@ -1827,89 +1846,96 @@
       <c r="B28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="50"/>
+      <c r="D28" s="64"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="48"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="54"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="57">
+      <c r="C32" s="61">
         <f>C6/'Financial Model'!O18</f>
         <v>-1.3734895864958347</v>
       </c>
-      <c r="D32" s="58"/>
+      <c r="D32" s="62"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="53">
+      <c r="C33" s="55">
         <f>C6/SUM('Financial Model'!N19:Q19)</f>
         <v>55.92365534541274</v>
       </c>
-      <c r="D33" s="54"/>
+      <c r="D33" s="56"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="52"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="60"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="53">
+      <c r="C35" s="55">
         <f>C6/'Financial Model'!Q64</f>
         <v>1.7061927095638381</v>
       </c>
-      <c r="D35" s="54"/>
+      <c r="D35" s="56"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="6"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="52"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="60"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="53">
+      <c r="C37" s="55">
         <f>C6/'Financial Model'!X19</f>
         <v>5.1256003193794974</v>
       </c>
-      <c r="D37" s="54"/>
+      <c r="D37" s="56"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="53">
+      <c r="C38" s="55">
         <f>C12/'Financial Model'!X18</f>
         <v>3.6900092011710619</v>
       </c>
-      <c r="D38" s="54"/>
+      <c r="D38" s="56"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="S5:W5"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
@@ -1926,13 +1952,6 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28:D28" r:id="rId1" display="Link" xr:uid="{D85FB78D-8AAC-49F6-8EB8-C86ABC1A5D8F}"/>
@@ -1951,14 +1970,16 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="R12" sqref="R12:R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="1"/>
     <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="17" width="9.1640625" style="1"/>
+    <col min="18" max="18" width="9.1640625" style="72"/>
+    <col min="19" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:35" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -2007,7 +2028,7 @@
       <c r="Q1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="65" t="s">
         <v>45</v>
       </c>
       <c r="U1" s="18" t="s">
@@ -2085,6 +2106,7 @@
       <c r="Q2" s="22">
         <v>44863</v>
       </c>
+      <c r="R2" s="66"/>
       <c r="V2" s="22">
         <v>43862</v>
       </c>
@@ -2096,7 +2118,7 @@
       </c>
     </row>
     <row r="3" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="51" t="s">
         <v>103</v>
       </c>
       <c r="H3" s="31">
@@ -2127,6 +2149,7 @@
       <c r="Q3" s="31">
         <v>457.75200000000001</v>
       </c>
+      <c r="R3" s="67"/>
       <c r="V3" s="31">
         <v>2158.5140000000001</v>
       </c>
@@ -2138,7 +2161,7 @@
       </c>
     </row>
     <row r="4" spans="2:35" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="51" t="s">
         <v>104</v>
       </c>
       <c r="H4" s="31">
@@ -2169,6 +2192,7 @@
       <c r="Q4" s="31">
         <v>422.33199999999999</v>
       </c>
+      <c r="R4" s="67"/>
       <c r="V4" s="31">
         <v>1464.559</v>
       </c>
@@ -2211,6 +2235,7 @@
       <c r="Q5" s="24">
         <v>880.08399999999995</v>
       </c>
+      <c r="R5" s="68"/>
       <c r="V5" s="24">
         <f>V3+V4</f>
         <v>3623.0730000000003</v>
@@ -2256,6 +2281,7 @@
       <c r="Q6" s="25">
         <v>359.26799999999997</v>
       </c>
+      <c r="R6" s="69"/>
       <c r="V6" s="25">
         <v>1472.155</v>
       </c>
@@ -2306,6 +2332,7 @@
         <f t="shared" si="1"/>
         <v>520.81600000000003</v>
       </c>
+      <c r="R7" s="68"/>
       <c r="V7" s="24">
         <f>V5-V6</f>
         <v>2150.9180000000006</v>
@@ -2351,6 +2378,7 @@
       <c r="Q8" s="25">
         <v>367.33300000000003</v>
       </c>
+      <c r="R8" s="69"/>
       <c r="V8" s="25">
         <v>1551.2429999999999</v>
       </c>
@@ -2393,6 +2421,7 @@
       <c r="Q9" s="25">
         <v>133.20099999999999</v>
       </c>
+      <c r="R9" s="69"/>
       <c r="V9" s="25">
         <v>464.61500000000001</v>
       </c>
@@ -2435,6 +2464,7 @@
       <c r="Q10" s="25">
         <v>3.7440000000000002</v>
       </c>
+      <c r="R10" s="69"/>
       <c r="V10" s="25">
         <v>19.135000000000002</v>
       </c>
@@ -2481,6 +2511,7 @@
       <c r="Q11" s="25">
         <v>-1.0049999999999999</v>
       </c>
+      <c r="R11" s="69"/>
       <c r="V11" s="25">
         <f>47.257-1.4</f>
         <v>45.856999999999999</v>
@@ -2534,6 +2565,10 @@
         <f t="shared" si="3"/>
         <v>17.54300000000001</v>
       </c>
+      <c r="R12" s="68">
+        <f>Q12+Q10</f>
+        <v>21.28700000000001</v>
+      </c>
       <c r="V12" s="24">
         <f>V7-V8-V9-V10-V11</f>
         <v>70.068000000000623</v>
@@ -2579,6 +2614,10 @@
       <c r="Q13" s="25">
         <v>7.2949999999999999</v>
       </c>
+      <c r="R13" s="69">
+        <f>Q13</f>
+        <v>7.2949999999999999</v>
+      </c>
       <c r="V13" s="25">
         <v>7.7370000000000001</v>
       </c>
@@ -2602,7 +2641,7 @@
         <v>49.807000000000038</v>
       </c>
       <c r="K14" s="25">
-        <f t="shared" ref="K14:Q14" si="4">K12-K13</f>
+        <f t="shared" ref="K14:R14" si="4">K12-K13</f>
         <v>48.82699999999997</v>
       </c>
       <c r="L14" s="25">
@@ -2629,6 +2668,10 @@
         <f t="shared" si="4"/>
         <v>10.24800000000001</v>
       </c>
+      <c r="R14" s="69">
+        <f t="shared" si="4"/>
+        <v>13.99200000000001</v>
+      </c>
       <c r="V14" s="25">
         <f>V12-V13</f>
         <v>62.331000000000621</v>
@@ -2674,6 +2717,9 @@
       <c r="Q15" s="25">
         <v>10.965999999999999</v>
       </c>
+      <c r="R15" s="69">
+        <v>11.942</v>
+      </c>
       <c r="V15" s="25">
         <v>17.370999999999999</v>
       </c>
@@ -2697,7 +2743,7 @@
         <v>44.028000000000034</v>
       </c>
       <c r="K16" s="24">
-        <f t="shared" ref="K16:Q16" si="5">K14-K15</f>
+        <f t="shared" ref="K16:R16" si="5">K14-K15</f>
         <v>42.705999999999968</v>
       </c>
       <c r="L16" s="24">
@@ -2724,6 +2770,10 @@
         <f t="shared" si="5"/>
         <v>-0.71799999999998931</v>
       </c>
+      <c r="R16" s="68">
+        <f>R14-R15</f>
+        <v>2.0500000000000096</v>
+      </c>
       <c r="V16" s="24">
         <f>V14-V15</f>
         <v>44.960000000000619</v>
@@ -2767,6 +2817,10 @@
         <v>2.0920000000000001</v>
       </c>
       <c r="Q17" s="25">
+        <v>1.496</v>
+      </c>
+      <c r="R17" s="69">
+        <f>Q17</f>
         <v>1.496</v>
       </c>
       <c r="V17" s="25">
@@ -2820,6 +2874,10 @@
         <f t="shared" si="6"/>
         <v>-2.2139999999999893</v>
       </c>
+      <c r="R18" s="68">
+        <f>R16-R17</f>
+        <v>0.5540000000000096</v>
+      </c>
       <c r="V18" s="24">
         <f>V16-V17</f>
         <v>39.358000000000615</v>
@@ -2874,6 +2932,10 @@
         <f t="shared" si="7"/>
         <v>-4.473992644384249E-2</v>
       </c>
+      <c r="R19" s="70">
+        <f>R18/R20</f>
+        <v>1.1195085478721448E-2</v>
+      </c>
       <c r="V19" s="23">
         <f>V18/V20</f>
         <v>0.61088346681567973</v>
@@ -2918,6 +2980,9 @@
         <v>50.441000000000003</v>
       </c>
       <c r="Q20" s="25">
+        <v>49.485999999999997</v>
+      </c>
+      <c r="R20" s="69">
         <v>49.485999999999997</v>
       </c>
       <c r="V20" s="29">
@@ -2956,6 +3021,7 @@
         <f t="shared" ref="Q22" si="9">Q5/M5-1</f>
         <v>-2.770338945600781E-2</v>
       </c>
+      <c r="R22" s="71"/>
       <c r="W22" s="28">
         <f>W5/V5-1</f>
         <v>-0.137366539399013</v>
@@ -3442,6 +3508,7 @@
       <c r="Q39" s="24">
         <v>257.33199999999999</v>
       </c>
+      <c r="R39" s="71"/>
       <c r="W39" s="24">
         <v>1104.8620000000001</v>
       </c>
@@ -3482,6 +3549,7 @@
       <c r="Q41" s="24">
         <v>741.96299999999997</v>
       </c>
+      <c r="R41" s="71"/>
       <c r="W41" s="24">
         <v>404.053</v>
       </c>
@@ -3811,6 +3879,7 @@
       <c r="Q55" s="24">
         <v>296.53199999999998</v>
       </c>
+      <c r="R55" s="71"/>
       <c r="W55" s="24">
         <v>343.91</v>
       </c>
@@ -3989,6 +4058,7 @@
       <c r="B66" s="3" t="s">
         <v>132</v>
       </c>
+      <c r="R66" s="71"/>
       <c r="X66" s="28">
         <f>X41/W41-1</f>
         <v>0.30147282658463137</v>
@@ -4008,7 +4078,7 @@
       </c>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A68" s="61">
+      <c r="A68" s="48">
         <f>AVERAGE( C68:AK68)</f>
         <v>0.25420875419415584</v>
       </c>
@@ -4028,7 +4098,7 @@
         <v>0.33349775502898105</v>
       </c>
       <c r="W68" s="26">
-        <f t="shared" ref="W68:X68" si="37">W41/W5</f>
+        <f t="shared" ref="W68" si="37">W41/W5</f>
         <v>0.12928107394163404</v>
       </c>
       <c r="X68" s="26">
@@ -4041,7 +4111,7 @@
         <v>6</v>
       </c>
       <c r="O70" s="31">
-        <f t="shared" ref="O70:Q70" si="38">O39</f>
+        <f t="shared" ref="O70:P70" si="38">O39</f>
         <v>468.37799999999999</v>
       </c>
       <c r="P70" s="31">
@@ -4052,6 +4122,7 @@
         <f>Q39</f>
         <v>257.33199999999999</v>
       </c>
+      <c r="R70" s="73"/>
       <c r="W70" s="31">
         <f>W39</f>
         <v>1104.8620000000001</v>
@@ -4066,7 +4137,7 @@
         <v>7</v>
       </c>
       <c r="O71" s="31">
-        <f t="shared" ref="O71:Q71" si="39">O55</f>
+        <f t="shared" ref="O71:P71" si="39">O55</f>
         <v>303.90100000000001</v>
       </c>
       <c r="P71" s="31">
@@ -4077,6 +4148,7 @@
         <f>Q55</f>
         <v>296.53199999999998</v>
       </c>
+      <c r="R71" s="73"/>
       <c r="W71" s="31">
         <f>W55</f>
         <v>343.91</v>
@@ -4115,6 +4187,7 @@
       <c r="B74" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="R74" s="71"/>
       <c r="X74" s="28">
         <f>X39/W39-1</f>
         <v>-0.25498478543021663</v>
@@ -4125,7 +4198,7 @@
         <v>135</v>
       </c>
       <c r="P75" s="26">
-        <f t="shared" ref="P75:Q75" si="41">P70/O70-1</f>
+        <f t="shared" ref="P75" si="41">P70/O70-1</f>
         <v>-0.21013369543402971</v>
       </c>
       <c r="Q75" s="26">
@@ -4209,122 +4282,122 @@
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A81" s="60">
+      <c r="A81" s="47">
         <f>AVERAGE( C81:AK81)</f>
         <v>1.797859412227653</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O81" s="59">
-        <f t="shared" ref="O81:Q81" si="46">O77/O64</f>
+      <c r="O81" s="46">
+        <f t="shared" ref="O81:P81" si="46">O77/O64</f>
         <v>2.5550651031136269</v>
       </c>
-      <c r="P81" s="59">
+      <c r="P81" s="46">
         <f t="shared" si="46"/>
         <v>1.2684166002829735</v>
       </c>
-      <c r="Q81" s="59">
+      <c r="Q81" s="46">
         <f>Q77/Q64</f>
         <v>1.3260330607485531</v>
       </c>
-      <c r="V81" s="59"/>
-      <c r="W81" s="59">
-        <f t="shared" ref="V81:X81" si="47">W77/W64</f>
+      <c r="V81" s="46"/>
+      <c r="W81" s="46">
+        <f t="shared" ref="W81" si="47">W77/W64</f>
         <v>1.3500614004226084</v>
       </c>
-      <c r="X81" s="59">
+      <c r="X81" s="46">
         <f>X77/X64</f>
         <v>2.4897208965705029</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A82" s="60">
+      <c r="A82" s="47">
         <f>AVERAGE( C82:AK82)</f>
         <v>0.3843875677046612</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="O82" s="59">
+      <c r="O82" s="46">
         <f t="shared" ref="O82:P82" si="48">O78/SUM(L5:O5)</f>
         <v>0.48097290021032946</v>
       </c>
-      <c r="P82" s="59">
+      <c r="P82" s="46">
         <f t="shared" si="48"/>
         <v>0.23164412004670545</v>
       </c>
-      <c r="Q82" s="59">
+      <c r="Q82" s="46">
         <f>Q78/SUM(N5:Q5)</f>
         <v>0.23774116836872725</v>
       </c>
-      <c r="W82" s="59">
+      <c r="W82" s="46">
         <f>W78/W5</f>
         <v>0.41008400567738235</v>
       </c>
-      <c r="X82" s="59">
+      <c r="X82" s="46">
         <f>X78/X5</f>
         <v>0.56149564422016129</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A83" s="60">
+      <c r="A83" s="47">
         <f>AVERAGE( C83:AK83)</f>
         <v>0.29749280159584623</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O83" s="59">
+      <c r="O83" s="46">
         <f t="shared" ref="O83:P83" si="49">O79/SUM(L5:O5)</f>
         <v>0.43704354421927688</v>
       </c>
-      <c r="P83" s="59">
+      <c r="P83" s="46">
         <f t="shared" si="49"/>
         <v>0.21380197298531148</v>
       </c>
-      <c r="Q83" s="59">
+      <c r="Q83" s="46">
         <f>Q79/SUM(N5:Q5)</f>
         <v>0.24845362898267145</v>
       </c>
-      <c r="W83" s="59">
-        <f t="shared" ref="W83:X83" si="50">W79/W5</f>
+      <c r="W83" s="46">
+        <f t="shared" ref="W83" si="50">W79/W5</f>
         <v>0.16660928385120033</v>
       </c>
-      <c r="X83" s="59">
+      <c r="X83" s="46">
         <f>X79/X5</f>
         <v>0.42155557794077081</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A84" s="60">
+      <c r="A84" s="47">
         <f>AVERAGE( C84:AK84)</f>
         <v>15.362787955012152</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O84" s="59">
+      <c r="O84" s="46">
         <f t="shared" ref="O84:P84" si="51">O77/SUM(L19:O19)</f>
         <v>10.314417228677181</v>
       </c>
-      <c r="P84" s="59">
+      <c r="P84" s="46">
         <f t="shared" si="51"/>
         <v>13.508368512238665</v>
       </c>
-      <c r="Q84" s="59">
+      <c r="Q84" s="46">
         <f>Q77/SUM(N19:Q19)</f>
         <v>43.463212244578067</v>
       </c>
-      <c r="V84" s="59">
-        <f t="shared" ref="V84:X84" si="52">V77/V19</f>
+      <c r="V84" s="46">
+        <f t="shared" ref="V84:W84" si="52">V77/V19</f>
         <v>28.205052085979538</v>
       </c>
-      <c r="W84" s="59">
+      <c r="W84" s="46">
         <f t="shared" si="52"/>
         <v>-11.240648564738059</v>
       </c>
-      <c r="X84" s="59">
+      <c r="X84" s="46">
         <f>X77/X19</f>
         <v>7.9263262233375249</v>
       </c>
@@ -4333,20 +4406,20 @@
       <c r="B85" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O85" s="59">
+      <c r="O85" s="46">
         <f t="shared" ref="O85:P85" si="53">O79/SUM(L16:O16)</f>
         <v>7.6999428743518044</v>
       </c>
-      <c r="P85" s="59">
+      <c r="P85" s="46">
         <f t="shared" si="53"/>
         <v>9.0215392367950873</v>
       </c>
-      <c r="Q85" s="59">
+      <c r="Q85" s="46">
         <f>Q79/SUM(N16:Q16)</f>
         <v>24.23144669509588</v>
       </c>
-      <c r="W85" s="59"/>
-      <c r="X85" s="59">
+      <c r="W85" s="46"/>
+      <c r="X85" s="46">
         <f>X79/X16</f>
         <v>5.7953909785015574</v>
       </c>
@@ -4380,27 +4453,34 @@
       <c r="Q93" s="24">
         <v>-301.19400000000002</v>
       </c>
-    </row>
-    <row r="94" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.15"/>
+      <c r="R93" s="68"/>
+    </row>
+    <row r="94" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="R94" s="69"/>
+    </row>
     <row r="95" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B95" s="25" t="s">
         <v>149</v>
       </c>
+      <c r="R95" s="69"/>
     </row>
     <row r="96" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B96" s="25" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="97" spans="2:2" s="25" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="R96" s="69"/>
+    </row>
+    <row r="97" spans="2:18" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B97" s="25" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" s="24" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="R97" s="69"/>
+    </row>
+    <row r="98" spans="2:18" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B98" s="24" t="s">
         <v>148</v>
       </c>
+      <c r="R98" s="68"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4413,7 +4493,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="N7 N15:N17 N14 N12" formula="1"/>
+    <ignoredError sqref="N7 N15:N17 N14 N12 R17" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId7"/>
 </worksheet>

</xml_diff>